<commit_message>
created encomienda endpoints, and work some about xlsx exports
</commit_message>
<xml_diff>
--- a/src/templates/TEMPLATEGUIA.xlsx
+++ b/src/templates/TEMPLATEGUIA.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24923"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC8E30DB-9FFC-4361-B1BD-5AAEF86560DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB51E435-0EE6-427B-AD0E-E0DB1D134578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hoja1" sheetId="2" r:id="rId1"/>
@@ -268,10 +268,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="41" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-[$$-240A]* #,##0_-;\-[$$-240A]* #,##0_-;_-[$$-240A]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$$-240A]* #,##0_-;\-[$$-240A]* #,##0_-;_-[$$-240A]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +347,14 @@
     <font>
       <sz val="6"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -535,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -570,13 +578,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -601,7 +609,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -673,6 +681,105 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -691,9 +798,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -775,125 +879,32 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -977,50 +988,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>750094</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>297656</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>130969</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>91737</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1352,101 +1319,101 @@
   <dimension ref="B1:AZ78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R61" sqref="R61:U61"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="6.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="3.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" style="1" customWidth="1"/>
-    <col min="14" max="16" width="2.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="4.5703125" style="1" customWidth="1"/>
-    <col min="19" max="21" width="2.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="6.7109375" style="1" customWidth="1"/>
-    <col min="24" max="26" width="4.85546875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="11.42578125" style="1" customWidth="1"/>
-    <col min="28" max="29" width="6.5703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="15.7109375" style="1" customWidth="1"/>
-    <col min="31" max="31" width="3.42578125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5703125" style="1" customWidth="1"/>
-    <col min="33" max="33" width="2.85546875" style="1" customWidth="1"/>
-    <col min="34" max="34" width="7.140625" style="1" customWidth="1"/>
-    <col min="35" max="35" width="6.85546875" style="1" customWidth="1"/>
-    <col min="36" max="36" width="17.28515625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="3.42578125" style="1" customWidth="1"/>
-    <col min="38" max="38" width="14.5703125" style="1" customWidth="1"/>
-    <col min="39" max="39" width="2.140625" style="1" customWidth="1"/>
-    <col min="40" max="42" width="2.7109375" style="1" customWidth="1"/>
-    <col min="43" max="43" width="7.140625" style="1" customWidth="1"/>
-    <col min="44" max="44" width="4.5703125" style="1" customWidth="1"/>
-    <col min="45" max="47" width="2.7109375" style="1" customWidth="1"/>
-    <col min="48" max="48" width="9.140625" style="1" customWidth="1"/>
-    <col min="49" max="49" width="6.7109375" style="1" customWidth="1"/>
-    <col min="50" max="52" width="4.85546875" style="1" customWidth="1"/>
-    <col min="53" max="53" width="11.42578125" style="1" customWidth="1"/>
-    <col min="54" max="55" width="6.5703125" style="1" customWidth="1"/>
-    <col min="56" max="56" width="15.7109375" style="1" customWidth="1"/>
-    <col min="57" max="57" width="3.42578125" style="1" customWidth="1"/>
-    <col min="58" max="58" width="12.7109375" style="1" customWidth="1"/>
-    <col min="59" max="59" width="7.140625" style="1" customWidth="1"/>
-    <col min="60" max="60" width="6.85546875" style="1" customWidth="1"/>
-    <col min="61" max="61" width="17.28515625" style="1" customWidth="1"/>
-    <col min="62" max="62" width="3.42578125" style="1" customWidth="1"/>
-    <col min="63" max="63" width="12.7109375" style="1" customWidth="1"/>
-    <col min="64" max="66" width="2.7109375" style="1" customWidth="1"/>
-    <col min="67" max="67" width="7.140625" style="1" customWidth="1"/>
-    <col min="68" max="68" width="4.5703125" style="1" customWidth="1"/>
-    <col min="69" max="71" width="2.7109375" style="1" customWidth="1"/>
-    <col min="72" max="72" width="9.140625" style="1" customWidth="1"/>
-    <col min="73" max="73" width="6.7109375" style="1" customWidth="1"/>
-    <col min="74" max="76" width="4.85546875" style="1" customWidth="1"/>
-    <col min="77" max="77" width="11.42578125" style="1" customWidth="1"/>
-    <col min="78" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="6.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="3.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="2.109375" style="1" customWidth="1"/>
+    <col min="14" max="16" width="2.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5546875" style="1" customWidth="1"/>
+    <col min="19" max="21" width="2.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="9.109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="6.6640625" style="1" customWidth="1"/>
+    <col min="24" max="26" width="4.88671875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="11.44140625" style="1" customWidth="1"/>
+    <col min="28" max="29" width="6.5546875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="3.44140625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5546875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="2.88671875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="7.109375" style="1" customWidth="1"/>
+    <col min="35" max="35" width="6.88671875" style="1" customWidth="1"/>
+    <col min="36" max="36" width="17.33203125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="3.44140625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="14.5546875" style="1" customWidth="1"/>
+    <col min="39" max="39" width="2.109375" style="1" customWidth="1"/>
+    <col min="40" max="42" width="2.6640625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="7.109375" style="1" customWidth="1"/>
+    <col min="44" max="44" width="4.5546875" style="1" customWidth="1"/>
+    <col min="45" max="47" width="2.6640625" style="1" customWidth="1"/>
+    <col min="48" max="48" width="9.109375" style="1" customWidth="1"/>
+    <col min="49" max="49" width="6.6640625" style="1" customWidth="1"/>
+    <col min="50" max="52" width="4.88671875" style="1" customWidth="1"/>
+    <col min="53" max="53" width="11.44140625" style="1" customWidth="1"/>
+    <col min="54" max="55" width="6.5546875" style="1" customWidth="1"/>
+    <col min="56" max="56" width="15.6640625" style="1" customWidth="1"/>
+    <col min="57" max="57" width="3.44140625" style="1" customWidth="1"/>
+    <col min="58" max="58" width="12.6640625" style="1" customWidth="1"/>
+    <col min="59" max="59" width="7.109375" style="1" customWidth="1"/>
+    <col min="60" max="60" width="6.88671875" style="1" customWidth="1"/>
+    <col min="61" max="61" width="17.33203125" style="1" customWidth="1"/>
+    <col min="62" max="62" width="3.44140625" style="1" customWidth="1"/>
+    <col min="63" max="63" width="12.6640625" style="1" customWidth="1"/>
+    <col min="64" max="66" width="2.6640625" style="1" customWidth="1"/>
+    <col min="67" max="67" width="7.109375" style="1" customWidth="1"/>
+    <col min="68" max="68" width="4.5546875" style="1" customWidth="1"/>
+    <col min="69" max="71" width="2.6640625" style="1" customWidth="1"/>
+    <col min="72" max="72" width="9.109375" style="1" customWidth="1"/>
+    <col min="73" max="73" width="6.6640625" style="1" customWidth="1"/>
+    <col min="74" max="76" width="4.88671875" style="1" customWidth="1"/>
+    <col min="77" max="77" width="11.44140625" style="1" customWidth="1"/>
+    <col min="78" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:52" ht="27.75" customHeight="1">
       <c r="V1" s="2"/>
     </row>
     <row r="2" spans="2:52">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="H2" s="92" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="H2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92" t="s">
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="92"/>
-      <c r="R2" s="92"/>
-      <c r="S2" s="92"/>
-      <c r="T2" s="92"/>
-      <c r="V2" s="92" t="s">
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="V2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="92"/>
-      <c r="X2" s="92"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
       <c r="AJ2" s="3"/>
@@ -1465,36 +1432,36 @@
       <c r="AX2" s="3"/>
     </row>
     <row r="3" spans="2:52" ht="15" customHeight="1">
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="H3" s="92" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="H3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="113" t="s">
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="113"/>
-      <c r="N3" s="113"/>
-      <c r="O3" s="113"/>
-      <c r="P3" s="113"/>
-      <c r="Q3" s="113"/>
-      <c r="R3" s="113"/>
-      <c r="S3" s="113"/>
-      <c r="T3" s="113"/>
-      <c r="U3" s="113"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="51"/>
+      <c r="U3" s="51"/>
       <c r="V3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="115">
+      <c r="W3" s="53">
         <v>10090</v>
       </c>
-      <c r="X3" s="115"/>
+      <c r="X3" s="53"/>
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
       <c r="AJ3" s="3"/>
@@ -1510,27 +1477,27 @@
       <c r="AX3" s="5"/>
     </row>
     <row r="4" spans="2:52" ht="15" customHeight="1">
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="H4" s="92" t="s">
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="H4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="113"/>
-      <c r="M4" s="113"/>
-      <c r="N4" s="113"/>
-      <c r="O4" s="113"/>
-      <c r="P4" s="113"/>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="113"/>
-      <c r="S4" s="113"/>
-      <c r="T4" s="113"/>
-      <c r="U4" s="113"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="51"/>
+      <c r="U4" s="51"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
@@ -1549,70 +1516,70 @@
       <c r="AX4" s="5"/>
     </row>
     <row r="5" spans="2:52" ht="15" customHeight="1">
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="H5" s="101" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="H5" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114"/>
-      <c r="P5" s="114"/>
-      <c r="Q5" s="114"/>
-      <c r="R5" s="114"/>
-      <c r="S5" s="114"/>
-      <c r="T5" s="114"/>
-      <c r="U5" s="114"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="52"/>
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
     </row>
     <row r="6" spans="2:52">
-      <c r="B6" s="116" t="s">
+      <c r="B6" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110" t="s">
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
       <c r="J6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="110" t="s">
+      <c r="K6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="110"/>
-      <c r="Q6" s="110"/>
-      <c r="R6" s="110"/>
-      <c r="S6" s="110"/>
-      <c r="T6" s="110"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="55"/>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="55"/>
       <c r="U6" s="7"/>
-      <c r="V6" s="111" t="s">
+      <c r="V6" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="W6" s="111"/>
-      <c r="X6" s="117" t="s">
+      <c r="W6" s="56"/>
+      <c r="X6" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="Y6" s="117"/>
-      <c r="Z6" s="118"/>
+      <c r="Y6" s="57"/>
+      <c r="Z6" s="58"/>
       <c r="AB6" s="8"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8"/>
@@ -1638,45 +1605,45 @@
       <c r="AZ6" s="9"/>
     </row>
     <row r="7" spans="2:52" ht="18.75" customHeight="1">
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="89"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="92"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="99" t="s">
+      <c r="K7" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="100"/>
-      <c r="P7" s="100"/>
-      <c r="Q7" s="100"/>
-      <c r="R7" s="100"/>
-      <c r="S7" s="100"/>
-      <c r="T7" s="100"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
       <c r="U7" s="11"/>
-      <c r="V7" s="101" t="s">
+      <c r="V7" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="101"/>
-      <c r="X7" s="102" t="s">
+      <c r="W7" s="50"/>
+      <c r="X7" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="Y7" s="102"/>
-      <c r="Z7" s="103"/>
+      <c r="Y7" s="63"/>
+      <c r="Z7" s="64"/>
       <c r="AB7" s="8"/>
       <c r="AC7" s="8"/>
       <c r="AH7" s="3"/>
@@ -1698,39 +1665,39 @@
       <c r="AZ7" s="12"/>
     </row>
     <row r="8" spans="2:52" ht="15" customHeight="1">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="104" t="s">
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="110" t="s">
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="110"/>
-      <c r="P8" s="110"/>
-      <c r="Q8" s="110"/>
-      <c r="R8" s="111" t="s">
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="S8" s="111"/>
-      <c r="T8" s="111"/>
-      <c r="U8" s="111"/>
-      <c r="V8" s="111"/>
-      <c r="W8" s="111"/>
-      <c r="X8" s="111"/>
-      <c r="Y8" s="111"/>
-      <c r="Z8" s="112"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="56"/>
+      <c r="U8" s="56"/>
+      <c r="V8" s="56"/>
+      <c r="W8" s="56"/>
+      <c r="X8" s="56"/>
+      <c r="Y8" s="56"/>
+      <c r="Z8" s="71"/>
       <c r="AB8" s="13"/>
       <c r="AC8" s="13"/>
       <c r="AD8" s="13"/>
@@ -1758,35 +1725,35 @@
       <c r="AZ8" s="3"/>
     </row>
     <row r="9" spans="2:52" ht="15" customHeight="1">
-      <c r="B9" s="107"/>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="107"/>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="108"/>
-      <c r="L9" s="108"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="89"/>
-      <c r="P9" s="89"/>
-      <c r="Q9" s="89"/>
-      <c r="R9" s="92"/>
-      <c r="S9" s="92"/>
-      <c r="T9" s="92"/>
-      <c r="U9" s="92"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="70"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
       <c r="V9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="W9" s="8"/>
-      <c r="X9" s="96" t="s">
+      <c r="X9" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="Y9" s="96"/>
-      <c r="Z9" s="97"/>
+      <c r="Y9" s="72"/>
+      <c r="Z9" s="73"/>
       <c r="AB9" s="13"/>
       <c r="AC9" s="13"/>
       <c r="AD9" s="13"/>
@@ -1814,39 +1781,39 @@
       <c r="AZ9" s="14"/>
     </row>
     <row r="10" spans="2:52" ht="15" customHeight="1">
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="87" t="s">
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="95"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
-      <c r="P10" s="89"/>
-      <c r="Q10" s="89"/>
-      <c r="R10" s="92"/>
-      <c r="S10" s="92"/>
-      <c r="T10" s="92"/>
-      <c r="U10" s="92"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="49"/>
+      <c r="U10" s="49"/>
       <c r="V10" s="8" t="s">
         <v>29</v>
       </c>
       <c r="W10" s="8"/>
-      <c r="X10" s="96" t="s">
+      <c r="X10" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="Y10" s="96"/>
-      <c r="Z10" s="97"/>
+      <c r="Y10" s="72"/>
+      <c r="Z10" s="73"/>
       <c r="AB10" s="15"/>
       <c r="AC10" s="15"/>
       <c r="AD10" s="15"/>
@@ -1874,35 +1841,35 @@
       <c r="AZ10" s="14"/>
     </row>
     <row r="11" spans="2:52" ht="15" customHeight="1">
-      <c r="B11" s="87"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="88"/>
-      <c r="L11" s="88"/>
-      <c r="M11" s="95"/>
-      <c r="N11" s="89"/>
-      <c r="O11" s="89"/>
-      <c r="P11" s="89"/>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="90"/>
-      <c r="T11" s="90"/>
-      <c r="U11" s="90"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="77"/>
+      <c r="S11" s="77"/>
+      <c r="T11" s="77"/>
+      <c r="U11" s="77"/>
       <c r="V11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="W11" s="8"/>
-      <c r="X11" s="96" t="s">
+      <c r="X11" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="Y11" s="96"/>
-      <c r="Z11" s="97"/>
+      <c r="Y11" s="72"/>
+      <c r="Z11" s="73"/>
       <c r="AB11" s="15"/>
       <c r="AC11" s="15"/>
       <c r="AD11" s="15"/>
@@ -1930,10 +1897,10 @@
       <c r="AZ11" s="14"/>
     </row>
     <row r="12" spans="2:52" ht="15" customHeight="1">
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="88"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="15">
         <v>3022053929</v>
       </c>
@@ -1946,10 +1913,10 @@
       <c r="G12" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="87" t="s">
+      <c r="H12" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="88"/>
+      <c r="I12" s="75"/>
       <c r="J12" s="15">
         <v>3022053929</v>
       </c>
@@ -1962,27 +1929,27 @@
       <c r="M12" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="89" t="s">
+      <c r="N12" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="89"/>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="96" t="s">
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="S12" s="96"/>
-      <c r="T12" s="96"/>
-      <c r="U12" s="96"/>
+      <c r="S12" s="72"/>
+      <c r="T12" s="72"/>
+      <c r="U12" s="72"/>
       <c r="V12" s="8" t="s">
         <v>35</v>
       </c>
       <c r="W12" s="8"/>
-      <c r="X12" s="90" t="s">
+      <c r="X12" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y12" s="90"/>
-      <c r="Z12" s="91"/>
+      <c r="Y12" s="77"/>
+      <c r="Z12" s="78"/>
       <c r="AB12" s="15"/>
       <c r="AC12" s="15"/>
       <c r="AD12" s="15"/>
@@ -2010,47 +1977,47 @@
       <c r="AZ12" s="16"/>
     </row>
     <row r="13" spans="2:52" ht="15" customHeight="1">
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88" t="s">
+      <c r="C13" s="75"/>
+      <c r="D13" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="87" t="s">
+      <c r="H13" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88" t="s">
+      <c r="I13" s="75"/>
+      <c r="J13" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="88"/>
-      <c r="L13" s="88"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
       <c r="M13" s="22"/>
-      <c r="N13" s="89" t="s">
+      <c r="N13" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="O13" s="89"/>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="90" t="s">
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="S13" s="90"/>
-      <c r="T13" s="90"/>
-      <c r="U13" s="90"/>
+      <c r="S13" s="77"/>
+      <c r="T13" s="77"/>
+      <c r="U13" s="77"/>
       <c r="V13" s="8" t="s">
         <v>40</v>
       </c>
       <c r="W13" s="8"/>
-      <c r="X13" s="90" t="s">
+      <c r="X13" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y13" s="90"/>
-      <c r="Z13" s="91"/>
+      <c r="Y13" s="77"/>
+      <c r="Z13" s="78"/>
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
       <c r="AD13" s="15"/>
@@ -2090,27 +2057,27 @@
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
       <c r="M14" s="22"/>
-      <c r="N14" s="89" t="s">
+      <c r="N14" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="O14" s="89"/>
-      <c r="P14" s="89"/>
-      <c r="Q14" s="89"/>
-      <c r="R14" s="90" t="s">
+      <c r="O14" s="60"/>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="60"/>
+      <c r="R14" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="S14" s="90"/>
-      <c r="T14" s="90"/>
-      <c r="U14" s="90"/>
+      <c r="S14" s="77"/>
+      <c r="T14" s="77"/>
+      <c r="U14" s="77"/>
       <c r="V14" s="8" t="s">
         <v>42</v>
       </c>
       <c r="W14" s="8"/>
-      <c r="X14" s="90" t="s">
+      <c r="X14" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y14" s="90"/>
-      <c r="Z14" s="91"/>
+      <c r="Y14" s="77"/>
+      <c r="Z14" s="78"/>
       <c r="AB14" s="17"/>
       <c r="AC14" s="17"/>
       <c r="AD14" s="17"/>
@@ -2138,47 +2105,47 @@
       <c r="AZ14" s="16"/>
     </row>
     <row r="15" spans="2:52" ht="15" customHeight="1">
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88" t="s">
+      <c r="C15" s="75"/>
+      <c r="D15" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
       <c r="G15" s="22"/>
-      <c r="H15" s="87" t="s">
+      <c r="H15" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88" t="s">
+      <c r="I15" s="75"/>
+      <c r="J15" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
+      <c r="K15" s="75"/>
+      <c r="L15" s="75"/>
       <c r="M15" s="22"/>
-      <c r="N15" s="89" t="s">
+      <c r="N15" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="89"/>
-      <c r="R15" s="90">
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="77">
         <v>0</v>
       </c>
-      <c r="S15" s="90"/>
-      <c r="T15" s="90"/>
-      <c r="U15" s="90"/>
+      <c r="S15" s="77"/>
+      <c r="T15" s="77"/>
+      <c r="U15" s="77"/>
       <c r="V15" s="8" t="s">
         <v>46</v>
       </c>
       <c r="W15" s="8"/>
-      <c r="X15" s="90" t="s">
+      <c r="X15" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y15" s="90"/>
-      <c r="Z15" s="91"/>
+      <c r="Y15" s="77"/>
+      <c r="Z15" s="78"/>
       <c r="AB15" s="15"/>
       <c r="AC15" s="15"/>
       <c r="AD15" s="15"/>
@@ -2218,23 +2185,23 @@
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
       <c r="M16" s="22"/>
-      <c r="N16" s="89"/>
-      <c r="O16" s="89"/>
-      <c r="P16" s="89"/>
-      <c r="Q16" s="89"/>
-      <c r="R16" s="92"/>
-      <c r="S16" s="92"/>
-      <c r="T16" s="92"/>
-      <c r="U16" s="92"/>
-      <c r="V16" s="55" t="s">
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+      <c r="U16" s="49"/>
+      <c r="V16" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="W16" s="55"/>
-      <c r="X16" s="93" t="s">
+      <c r="W16" s="79"/>
+      <c r="X16" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="Y16" s="93"/>
-      <c r="Z16" s="94"/>
+      <c r="Y16" s="80"/>
+      <c r="Z16" s="81"/>
       <c r="AB16" s="17"/>
       <c r="AC16" s="17"/>
       <c r="AD16" s="17"/>
@@ -2262,20 +2229,20 @@
       <c r="AZ16" s="25"/>
     </row>
     <row r="17" spans="2:52" ht="15" customHeight="1">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="50"/>
+      <c r="C17" s="83"/>
       <c r="D17" s="26" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49" t="s">
+      <c r="H17" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="50"/>
+      <c r="I17" s="83"/>
       <c r="J17" s="26" t="s">
         <v>49</v>
       </c>
@@ -2288,17 +2255,17 @@
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
-      <c r="R17" s="51" t="s">
+      <c r="R17" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="S17" s="51"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="51"/>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="51"/>
-      <c r="Z17" s="52"/>
+      <c r="S17" s="84"/>
+      <c r="T17" s="84"/>
+      <c r="U17" s="84"/>
+      <c r="V17" s="84"/>
+      <c r="W17" s="84"/>
+      <c r="X17" s="84"/>
+      <c r="Y17" s="84"/>
+      <c r="Z17" s="85"/>
       <c r="AB17" s="15"/>
       <c r="AC17" s="15"/>
       <c r="AD17" s="29"/>
@@ -2322,35 +2289,35 @@
       <c r="AZ17" s="8"/>
     </row>
     <row r="18" spans="2:52">
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="57" t="s">
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="O18" s="58"/>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="58"/>
-      <c r="S18" s="58"/>
-      <c r="T18" s="58"/>
-      <c r="U18" s="58"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="58"/>
-      <c r="X18" s="58"/>
-      <c r="Y18" s="58"/>
-      <c r="Z18" s="59"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="90"/>
+      <c r="Q18" s="90"/>
+      <c r="R18" s="90"/>
+      <c r="S18" s="90"/>
+      <c r="T18" s="90"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="90"/>
+      <c r="W18" s="90"/>
+      <c r="X18" s="90"/>
+      <c r="Y18" s="90"/>
+      <c r="Z18" s="91"/>
       <c r="AB18" s="24"/>
       <c r="AC18" s="24"/>
       <c r="AD18" s="24"/>
@@ -2378,20 +2345,20 @@
       <c r="AZ18" s="3"/>
     </row>
     <row r="19" spans="2:52" ht="18" customHeight="1">
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="62"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="93"/>
+      <c r="L19" s="93"/>
+      <c r="M19" s="94"/>
       <c r="N19" s="31">
         <v>1</v>
       </c>
@@ -2401,10 +2368,10 @@
       <c r="P19" s="31">
         <v>3</v>
       </c>
-      <c r="Q19" s="66" t="s">
+      <c r="Q19" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="R19" s="67"/>
+      <c r="R19" s="99"/>
       <c r="S19" s="31">
         <v>1</v>
       </c>
@@ -2456,18 +2423,18 @@
       <c r="AZ19" s="33"/>
     </row>
     <row r="20" spans="2:52" ht="18" customHeight="1">
-      <c r="B20" s="63"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="65"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="96"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="96"/>
+      <c r="L20" s="96"/>
+      <c r="M20" s="97"/>
       <c r="N20" s="31">
         <v>1</v>
       </c>
@@ -2477,10 +2444,10 @@
       <c r="P20" s="31">
         <v>3</v>
       </c>
-      <c r="Q20" s="66" t="s">
+      <c r="Q20" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="R20" s="67"/>
+      <c r="R20" s="99"/>
       <c r="S20" s="31">
         <v>1</v>
       </c>
@@ -2524,22 +2491,22 @@
       <c r="AZ20" s="34"/>
     </row>
     <row r="21" spans="2:52" ht="18" customHeight="1">
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="68"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="69" t="s">
+      <c r="C21" s="100"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="70"/>
-      <c r="J21" s="70"/>
-      <c r="K21" s="70"/>
-      <c r="L21" s="70"/>
-      <c r="M21" s="71"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="102"/>
+      <c r="J21" s="102"/>
+      <c r="K21" s="102"/>
+      <c r="L21" s="102"/>
+      <c r="M21" s="103"/>
       <c r="N21" s="31">
         <v>1</v>
       </c>
@@ -2549,10 +2516,10 @@
       <c r="P21" s="31">
         <v>3</v>
       </c>
-      <c r="Q21" s="75" t="s">
+      <c r="Q21" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="R21" s="75"/>
+      <c r="R21" s="107"/>
       <c r="S21" s="31">
         <v>1</v>
       </c>
@@ -2596,18 +2563,18 @@
       <c r="AZ21" s="34"/>
     </row>
     <row r="22" spans="2:52" ht="18" customHeight="1">
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="74"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="105"/>
+      <c r="J22" s="105"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="106"/>
       <c r="N22" s="36">
         <v>1</v>
       </c>
@@ -2617,10 +2584,10 @@
       <c r="P22" s="36">
         <v>3</v>
       </c>
-      <c r="Q22" s="76" t="s">
+      <c r="Q22" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="R22" s="76"/>
+      <c r="R22" s="108"/>
       <c r="S22" s="36">
         <v>1</v>
       </c>
@@ -2664,33 +2631,33 @@
       <c r="AZ22" s="34"/>
     </row>
     <row r="23" spans="2:52" ht="15" customHeight="1">
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="77" t="s">
+      <c r="B23" s="100"/>
+      <c r="C23" s="100"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="105"/>
+      <c r="J23" s="105"/>
+      <c r="K23" s="105"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="106"/>
+      <c r="N23" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="78"/>
-      <c r="P23" s="78"/>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="78"/>
-      <c r="S23" s="78"/>
-      <c r="T23" s="78"/>
-      <c r="U23" s="78"/>
-      <c r="V23" s="78"/>
-      <c r="W23" s="78"/>
-      <c r="X23" s="78"/>
-      <c r="Y23" s="78"/>
-      <c r="Z23" s="79"/>
+      <c r="O23" s="110"/>
+      <c r="P23" s="110"/>
+      <c r="Q23" s="110"/>
+      <c r="R23" s="110"/>
+      <c r="S23" s="110"/>
+      <c r="T23" s="110"/>
+      <c r="U23" s="110"/>
+      <c r="V23" s="110"/>
+      <c r="W23" s="110"/>
+      <c r="X23" s="110"/>
+      <c r="Y23" s="110"/>
+      <c r="Z23" s="111"/>
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
@@ -2718,18 +2685,18 @@
       <c r="AZ23" s="38"/>
     </row>
     <row r="24" spans="2:52" ht="15" customHeight="1">
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
-      <c r="M24" s="74"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="100"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="105"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="106"/>
       <c r="N24" s="39"/>
       <c r="O24" s="40"/>
       <c r="P24" s="40"/>
@@ -2776,18 +2743,18 @@
       <c r="AZ24" s="42"/>
     </row>
     <row r="25" spans="2:52">
-      <c r="B25" s="68"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="74"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="104"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="105"/>
+      <c r="I25" s="105"/>
+      <c r="J25" s="105"/>
+      <c r="K25" s="105"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="106"/>
       <c r="N25" s="39"/>
       <c r="O25" s="40"/>
       <c r="P25" s="40"/>
@@ -2798,11 +2765,11 @@
       <c r="U25" s="40"/>
       <c r="V25" s="40"/>
       <c r="W25" s="40"/>
-      <c r="X25" s="80" t="s">
+      <c r="X25" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="Y25" s="80"/>
-      <c r="Z25" s="80"/>
+      <c r="Y25" s="112"/>
+      <c r="Z25" s="112"/>
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
@@ -2830,32 +2797,32 @@
       <c r="AZ25" s="42"/>
     </row>
     <row r="26" spans="2:52" ht="15" customHeight="1">
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="82"/>
-      <c r="G26" s="82"/>
-      <c r="H26" s="82"/>
-      <c r="I26" s="121" t="s">
+      <c r="B26" s="100"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="113"/>
+      <c r="F26" s="114"/>
+      <c r="G26" s="114"/>
+      <c r="H26" s="114"/>
+      <c r="I26" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="J26" s="122"/>
-      <c r="K26" s="82"/>
-      <c r="L26" s="82"/>
+      <c r="J26" s="116"/>
+      <c r="K26" s="114"/>
+      <c r="L26" s="114"/>
       <c r="M26" s="44"/>
-      <c r="N26" s="85" t="s">
+      <c r="N26" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="O26" s="86"/>
-      <c r="P26" s="86"/>
-      <c r="Q26" s="86"/>
-      <c r="R26" s="86"/>
-      <c r="S26" s="86"/>
-      <c r="T26" s="86"/>
-      <c r="U26" s="86"/>
-      <c r="V26" s="86"/>
-      <c r="W26" s="86"/>
+      <c r="O26" s="118"/>
+      <c r="P26" s="118"/>
+      <c r="Q26" s="118"/>
+      <c r="R26" s="118"/>
+      <c r="S26" s="118"/>
+      <c r="T26" s="118"/>
+      <c r="U26" s="118"/>
+      <c r="V26" s="118"/>
+      <c r="W26" s="118"/>
       <c r="X26" s="45"/>
       <c r="Y26" s="45"/>
       <c r="Z26" s="46"/>
@@ -2887,28 +2854,28 @@
     </row>
     <row r="27" spans="2:52" ht="27.75" customHeight="1"/>
     <row r="28" spans="2:52" ht="15" customHeight="1">
-      <c r="H28" s="92" t="s">
+      <c r="H28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="I28" s="92"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="92"/>
-      <c r="L28" s="92" t="s">
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="M28" s="92"/>
-      <c r="N28" s="92"/>
-      <c r="O28" s="92"/>
-      <c r="P28" s="92"/>
-      <c r="Q28" s="92"/>
-      <c r="R28" s="92"/>
-      <c r="S28" s="92"/>
-      <c r="T28" s="92"/>
-      <c r="V28" s="92" t="s">
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="49"/>
+      <c r="V28" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="W28" s="92"/>
-      <c r="X28" s="92"/>
+      <c r="W28" s="49"/>
+      <c r="X28" s="49"/>
       <c r="AH28" s="3"/>
       <c r="AI28" s="3"/>
       <c r="AJ28" s="3"/>
@@ -2927,31 +2894,31 @@
       <c r="AX28" s="3"/>
     </row>
     <row r="29" spans="2:52" ht="15" customHeight="1">
-      <c r="H29" s="92" t="s">
+      <c r="H29" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="92"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="92"/>
-      <c r="L29" s="113" t="s">
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="M29" s="113"/>
-      <c r="N29" s="113"/>
-      <c r="O29" s="113"/>
-      <c r="P29" s="113"/>
-      <c r="Q29" s="113"/>
-      <c r="R29" s="113"/>
-      <c r="S29" s="113"/>
-      <c r="T29" s="113"/>
-      <c r="U29" s="113"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="51"/>
+      <c r="S29" s="51"/>
+      <c r="T29" s="51"/>
+      <c r="U29" s="51"/>
       <c r="V29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="W29" s="115">
+      <c r="W29" s="53">
         <v>10090</v>
       </c>
-      <c r="X29" s="115"/>
+      <c r="X29" s="53"/>
       <c r="AH29" s="3"/>
       <c r="AI29" s="3"/>
       <c r="AJ29" s="3"/>
@@ -2967,22 +2934,22 @@
       <c r="AX29" s="5"/>
     </row>
     <row r="30" spans="2:52" ht="15" customHeight="1">
-      <c r="H30" s="92" t="s">
+      <c r="H30" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="I30" s="92"/>
-      <c r="J30" s="92"/>
-      <c r="K30" s="92"/>
-      <c r="L30" s="113"/>
-      <c r="M30" s="113"/>
-      <c r="N30" s="113"/>
-      <c r="O30" s="113"/>
-      <c r="P30" s="113"/>
-      <c r="Q30" s="113"/>
-      <c r="R30" s="113"/>
-      <c r="S30" s="113"/>
-      <c r="T30" s="113"/>
-      <c r="U30" s="113"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="51"/>
+      <c r="T30" s="51"/>
+      <c r="U30" s="51"/>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
       <c r="X30" s="6"/>
@@ -3001,65 +2968,65 @@
       <c r="AX30" s="5"/>
     </row>
     <row r="31" spans="2:52">
-      <c r="H31" s="101" t="s">
+      <c r="H31" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="101"/>
-      <c r="J31" s="101"/>
-      <c r="K31" s="101"/>
-      <c r="L31" s="114"/>
-      <c r="M31" s="114"/>
-      <c r="N31" s="114"/>
-      <c r="O31" s="114"/>
-      <c r="P31" s="114"/>
-      <c r="Q31" s="114"/>
-      <c r="R31" s="114"/>
-      <c r="S31" s="114"/>
-      <c r="T31" s="114"/>
-      <c r="U31" s="114"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="52"/>
+      <c r="O31" s="52"/>
+      <c r="P31" s="52"/>
+      <c r="Q31" s="52"/>
+      <c r="R31" s="52"/>
+      <c r="S31" s="52"/>
+      <c r="T31" s="52"/>
+      <c r="U31" s="52"/>
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
       <c r="AJ31" s="3"/>
       <c r="AK31" s="3"/>
     </row>
     <row r="32" spans="2:52">
-      <c r="B32" s="116" t="s">
+      <c r="B32" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="110"/>
-      <c r="D32" s="110"/>
-      <c r="E32" s="110" t="s">
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="110"/>
-      <c r="G32" s="110"/>
-      <c r="H32" s="110"/>
-      <c r="I32" s="110"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
       <c r="J32" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K32" s="110" t="s">
+      <c r="K32" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="L32" s="110"/>
-      <c r="M32" s="110"/>
-      <c r="N32" s="110"/>
-      <c r="O32" s="110"/>
-      <c r="P32" s="110"/>
-      <c r="Q32" s="110"/>
-      <c r="R32" s="110"/>
-      <c r="S32" s="110"/>
-      <c r="T32" s="110"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="55"/>
+      <c r="N32" s="55"/>
+      <c r="O32" s="55"/>
+      <c r="P32" s="55"/>
+      <c r="Q32" s="55"/>
+      <c r="R32" s="55"/>
+      <c r="S32" s="55"/>
+      <c r="T32" s="55"/>
       <c r="U32" s="7"/>
-      <c r="V32" s="111" t="s">
+      <c r="V32" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="W32" s="111"/>
-      <c r="X32" s="117" t="s">
+      <c r="W32" s="56"/>
+      <c r="X32" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="Y32" s="117"/>
-      <c r="Z32" s="118"/>
+      <c r="Y32" s="57"/>
+      <c r="Z32" s="58"/>
       <c r="AB32" s="8"/>
       <c r="AC32" s="8"/>
       <c r="AD32" s="8"/>
@@ -3085,45 +3052,45 @@
       <c r="AZ32" s="9"/>
     </row>
     <row r="33" spans="2:52" ht="18.75" customHeight="1">
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="89"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="92" t="s">
+      <c r="H33" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="92"/>
+      <c r="I33" s="49"/>
       <c r="J33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="99" t="s">
+      <c r="K33" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="L33" s="99"/>
-      <c r="M33" s="99"/>
-      <c r="N33" s="100"/>
-      <c r="O33" s="100"/>
-      <c r="P33" s="100"/>
-      <c r="Q33" s="100"/>
-      <c r="R33" s="100"/>
-      <c r="S33" s="100"/>
-      <c r="T33" s="100"/>
+      <c r="L33" s="61"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="62"/>
+      <c r="P33" s="62"/>
+      <c r="Q33" s="62"/>
+      <c r="R33" s="62"/>
+      <c r="S33" s="62"/>
+      <c r="T33" s="62"/>
       <c r="U33" s="11"/>
-      <c r="V33" s="101" t="s">
+      <c r="V33" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="W33" s="101"/>
-      <c r="X33" s="102" t="s">
+      <c r="W33" s="50"/>
+      <c r="X33" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="Y33" s="102"/>
-      <c r="Z33" s="103"/>
+      <c r="Y33" s="63"/>
+      <c r="Z33" s="64"/>
       <c r="AB33" s="8"/>
       <c r="AC33" s="8"/>
       <c r="AH33" s="3"/>
@@ -3145,39 +3112,39 @@
       <c r="AZ33" s="12"/>
     </row>
     <row r="34" spans="2:52" ht="15" customHeight="1">
-      <c r="B34" s="104" t="s">
+      <c r="B34" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="105"/>
-      <c r="D34" s="105"/>
-      <c r="E34" s="105"/>
-      <c r="F34" s="105"/>
-      <c r="G34" s="106"/>
-      <c r="H34" s="104" t="s">
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="I34" s="105"/>
-      <c r="J34" s="105"/>
-      <c r="K34" s="105"/>
-      <c r="L34" s="105"/>
-      <c r="M34" s="106"/>
-      <c r="N34" s="110" t="s">
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="O34" s="110"/>
-      <c r="P34" s="110"/>
-      <c r="Q34" s="110"/>
-      <c r="R34" s="111" t="s">
+      <c r="O34" s="55"/>
+      <c r="P34" s="55"/>
+      <c r="Q34" s="55"/>
+      <c r="R34" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="S34" s="111"/>
-      <c r="T34" s="111"/>
-      <c r="U34" s="111"/>
-      <c r="V34" s="111"/>
-      <c r="W34" s="111"/>
-      <c r="X34" s="111"/>
-      <c r="Y34" s="111"/>
-      <c r="Z34" s="112"/>
+      <c r="S34" s="56"/>
+      <c r="T34" s="56"/>
+      <c r="U34" s="56"/>
+      <c r="V34" s="56"/>
+      <c r="W34" s="56"/>
+      <c r="X34" s="56"/>
+      <c r="Y34" s="56"/>
+      <c r="Z34" s="71"/>
       <c r="AB34" s="13"/>
       <c r="AC34" s="13"/>
       <c r="AD34" s="13"/>
@@ -3205,35 +3172,35 @@
       <c r="AZ34" s="3"/>
     </row>
     <row r="35" spans="2:52" ht="15" customHeight="1">
-      <c r="B35" s="107"/>
-      <c r="C35" s="108"/>
-      <c r="D35" s="108"/>
-      <c r="E35" s="108"/>
-      <c r="F35" s="108"/>
-      <c r="G35" s="109"/>
-      <c r="H35" s="107"/>
-      <c r="I35" s="108"/>
-      <c r="J35" s="108"/>
-      <c r="K35" s="108"/>
-      <c r="L35" s="108"/>
-      <c r="M35" s="109"/>
-      <c r="N35" s="89"/>
-      <c r="O35" s="89"/>
-      <c r="P35" s="89"/>
-      <c r="Q35" s="89"/>
-      <c r="R35" s="92"/>
-      <c r="S35" s="92"/>
-      <c r="T35" s="92"/>
-      <c r="U35" s="92"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="70"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="49"/>
+      <c r="U35" s="49"/>
       <c r="V35" s="8" t="s">
         <v>26</v>
       </c>
       <c r="W35" s="8"/>
-      <c r="X35" s="96" t="s">
+      <c r="X35" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="Y35" s="96"/>
-      <c r="Z35" s="97"/>
+      <c r="Y35" s="72"/>
+      <c r="Z35" s="73"/>
       <c r="AB35" s="13"/>
       <c r="AC35" s="13"/>
       <c r="AD35" s="13"/>
@@ -3261,39 +3228,39 @@
       <c r="AZ35" s="14"/>
     </row>
     <row r="36" spans="2:52" ht="15" customHeight="1">
-      <c r="B36" s="87" t="s">
+      <c r="B36" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="88"/>
-      <c r="D36" s="88"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="87" t="s">
+      <c r="C36" s="75"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="I36" s="88"/>
-      <c r="J36" s="88"/>
-      <c r="K36" s="88"/>
-      <c r="L36" s="88"/>
-      <c r="M36" s="95"/>
-      <c r="N36" s="89"/>
-      <c r="O36" s="89"/>
-      <c r="P36" s="89"/>
-      <c r="Q36" s="89"/>
-      <c r="R36" s="92"/>
-      <c r="S36" s="92"/>
-      <c r="T36" s="92"/>
-      <c r="U36" s="92"/>
+      <c r="I36" s="75"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="75"/>
+      <c r="L36" s="75"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="49"/>
+      <c r="U36" s="49"/>
       <c r="V36" s="8" t="s">
         <v>29</v>
       </c>
       <c r="W36" s="8"/>
-      <c r="X36" s="96" t="s">
+      <c r="X36" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="Y36" s="96"/>
-      <c r="Z36" s="97"/>
+      <c r="Y36" s="72"/>
+      <c r="Z36" s="73"/>
       <c r="AB36" s="15"/>
       <c r="AC36" s="15"/>
       <c r="AD36" s="15"/>
@@ -3321,35 +3288,35 @@
       <c r="AZ36" s="14"/>
     </row>
     <row r="37" spans="2:52" ht="15" customHeight="1">
-      <c r="B37" s="87"/>
-      <c r="C37" s="88"/>
-      <c r="D37" s="88"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="88"/>
-      <c r="G37" s="95"/>
-      <c r="H37" s="87"/>
-      <c r="I37" s="88"/>
-      <c r="J37" s="88"/>
-      <c r="K37" s="88"/>
-      <c r="L37" s="88"/>
-      <c r="M37" s="95"/>
-      <c r="N37" s="89"/>
-      <c r="O37" s="89"/>
-      <c r="P37" s="89"/>
-      <c r="Q37" s="89"/>
-      <c r="R37" s="90"/>
-      <c r="S37" s="90"/>
-      <c r="T37" s="90"/>
-      <c r="U37" s="90"/>
+      <c r="B37" s="74"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="77"/>
+      <c r="S37" s="77"/>
+      <c r="T37" s="77"/>
+      <c r="U37" s="77"/>
       <c r="V37" s="8" t="s">
         <v>30</v>
       </c>
       <c r="W37" s="8"/>
-      <c r="X37" s="96" t="s">
+      <c r="X37" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="Y37" s="96"/>
-      <c r="Z37" s="97"/>
+      <c r="Y37" s="72"/>
+      <c r="Z37" s="73"/>
       <c r="AB37" s="15"/>
       <c r="AC37" s="15"/>
       <c r="AD37" s="15"/>
@@ -3377,10 +3344,10 @@
       <c r="AZ37" s="14"/>
     </row>
     <row r="38" spans="2:52" ht="15" customHeight="1">
-      <c r="B38" s="87" t="s">
+      <c r="B38" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="88"/>
+      <c r="C38" s="75"/>
       <c r="D38" s="15">
         <v>3022053929</v>
       </c>
@@ -3393,10 +3360,10 @@
       <c r="G38" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H38" s="87" t="s">
+      <c r="H38" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="88"/>
+      <c r="I38" s="75"/>
       <c r="J38" s="15">
         <v>3022053929</v>
       </c>
@@ -3409,27 +3376,27 @@
       <c r="M38" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="N38" s="89" t="s">
+      <c r="N38" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="O38" s="89"/>
-      <c r="P38" s="89"/>
-      <c r="Q38" s="89"/>
-      <c r="R38" s="96" t="s">
+      <c r="O38" s="60"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="S38" s="96"/>
-      <c r="T38" s="96"/>
-      <c r="U38" s="96"/>
+      <c r="S38" s="72"/>
+      <c r="T38" s="72"/>
+      <c r="U38" s="72"/>
       <c r="V38" s="8" t="s">
         <v>35</v>
       </c>
       <c r="W38" s="8"/>
-      <c r="X38" s="90" t="s">
+      <c r="X38" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y38" s="90"/>
-      <c r="Z38" s="91"/>
+      <c r="Y38" s="77"/>
+      <c r="Z38" s="78"/>
       <c r="AB38" s="15"/>
       <c r="AC38" s="15"/>
       <c r="AD38" s="15"/>
@@ -3457,47 +3424,47 @@
       <c r="AZ38" s="16"/>
     </row>
     <row r="39" spans="2:52" ht="15" customHeight="1">
-      <c r="B39" s="87" t="s">
+      <c r="B39" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="88"/>
-      <c r="D39" s="88" t="s">
+      <c r="C39" s="75"/>
+      <c r="D39" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="88"/>
-      <c r="F39" s="88"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
       <c r="G39" s="22"/>
-      <c r="H39" s="87" t="s">
+      <c r="H39" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="88"/>
-      <c r="J39" s="88" t="s">
+      <c r="I39" s="75"/>
+      <c r="J39" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="K39" s="88"/>
-      <c r="L39" s="88"/>
+      <c r="K39" s="75"/>
+      <c r="L39" s="75"/>
       <c r="M39" s="22"/>
-      <c r="N39" s="89" t="s">
+      <c r="N39" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="O39" s="89"/>
-      <c r="P39" s="89"/>
-      <c r="Q39" s="89"/>
-      <c r="R39" s="90" t="s">
+      <c r="O39" s="60"/>
+      <c r="P39" s="60"/>
+      <c r="Q39" s="60"/>
+      <c r="R39" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="S39" s="90"/>
-      <c r="T39" s="90"/>
-      <c r="U39" s="90"/>
+      <c r="S39" s="77"/>
+      <c r="T39" s="77"/>
+      <c r="U39" s="77"/>
       <c r="V39" s="8" t="s">
         <v>40</v>
       </c>
       <c r="W39" s="8"/>
-      <c r="X39" s="90" t="s">
+      <c r="X39" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y39" s="90"/>
-      <c r="Z39" s="91"/>
+      <c r="Y39" s="77"/>
+      <c r="Z39" s="78"/>
       <c r="AB39" s="15"/>
       <c r="AC39" s="15"/>
       <c r="AD39" s="15"/>
@@ -3537,27 +3504,27 @@
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
       <c r="M40" s="22"/>
-      <c r="N40" s="89" t="s">
+      <c r="N40" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="O40" s="89"/>
-      <c r="P40" s="89"/>
-      <c r="Q40" s="89"/>
-      <c r="R40" s="90" t="s">
+      <c r="O40" s="60"/>
+      <c r="P40" s="60"/>
+      <c r="Q40" s="60"/>
+      <c r="R40" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="S40" s="90"/>
-      <c r="T40" s="90"/>
-      <c r="U40" s="90"/>
+      <c r="S40" s="77"/>
+      <c r="T40" s="77"/>
+      <c r="U40" s="77"/>
       <c r="V40" s="8" t="s">
         <v>42</v>
       </c>
       <c r="W40" s="8"/>
-      <c r="X40" s="90" t="s">
+      <c r="X40" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y40" s="90"/>
-      <c r="Z40" s="91"/>
+      <c r="Y40" s="77"/>
+      <c r="Z40" s="78"/>
       <c r="AB40" s="17"/>
       <c r="AC40" s="17"/>
       <c r="AD40" s="17"/>
@@ -3585,47 +3552,47 @@
       <c r="AZ40" s="16"/>
     </row>
     <row r="41" spans="2:52" ht="15" customHeight="1">
-      <c r="B41" s="87" t="s">
+      <c r="B41" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="88"/>
-      <c r="D41" s="88" t="s">
+      <c r="C41" s="75"/>
+      <c r="D41" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="88"/>
-      <c r="F41" s="88"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="75"/>
       <c r="G41" s="22"/>
-      <c r="H41" s="87" t="s">
+      <c r="H41" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="I41" s="88"/>
-      <c r="J41" s="88" t="s">
+      <c r="I41" s="75"/>
+      <c r="J41" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="K41" s="88"/>
-      <c r="L41" s="88"/>
+      <c r="K41" s="75"/>
+      <c r="L41" s="75"/>
       <c r="M41" s="22"/>
-      <c r="N41" s="89" t="s">
+      <c r="N41" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="O41" s="89"/>
-      <c r="P41" s="89"/>
-      <c r="Q41" s="89"/>
-      <c r="R41" s="90">
+      <c r="O41" s="60"/>
+      <c r="P41" s="60"/>
+      <c r="Q41" s="60"/>
+      <c r="R41" s="77">
         <v>0</v>
       </c>
-      <c r="S41" s="90"/>
-      <c r="T41" s="90"/>
-      <c r="U41" s="90"/>
+      <c r="S41" s="77"/>
+      <c r="T41" s="77"/>
+      <c r="U41" s="77"/>
       <c r="V41" s="8" t="s">
         <v>46</v>
       </c>
       <c r="W41" s="8"/>
-      <c r="X41" s="90" t="s">
+      <c r="X41" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y41" s="90"/>
-      <c r="Z41" s="91"/>
+      <c r="Y41" s="77"/>
+      <c r="Z41" s="78"/>
       <c r="AB41" s="15"/>
       <c r="AC41" s="15"/>
       <c r="AD41" s="15"/>
@@ -3665,23 +3632,23 @@
       <c r="K42" s="17"/>
       <c r="L42" s="17"/>
       <c r="M42" s="22"/>
-      <c r="N42" s="89"/>
-      <c r="O42" s="89"/>
-      <c r="P42" s="89"/>
-      <c r="Q42" s="89"/>
-      <c r="R42" s="92"/>
-      <c r="S42" s="92"/>
-      <c r="T42" s="92"/>
-      <c r="U42" s="92"/>
-      <c r="V42" s="55" t="s">
+      <c r="N42" s="60"/>
+      <c r="O42" s="60"/>
+      <c r="P42" s="60"/>
+      <c r="Q42" s="60"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="49"/>
+      <c r="U42" s="49"/>
+      <c r="V42" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="W42" s="55"/>
-      <c r="X42" s="93" t="s">
+      <c r="W42" s="79"/>
+      <c r="X42" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="Y42" s="93"/>
-      <c r="Z42" s="94"/>
+      <c r="Y42" s="80"/>
+      <c r="Z42" s="81"/>
       <c r="AB42" s="17"/>
       <c r="AC42" s="17"/>
       <c r="AD42" s="17"/>
@@ -3709,20 +3676,20 @@
       <c r="AZ42" s="25"/>
     </row>
     <row r="43" spans="2:52" ht="15" customHeight="1">
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="50"/>
+      <c r="C43" s="83"/>
       <c r="D43" s="26" t="s">
         <v>49</v>
       </c>
       <c r="E43" s="27"/>
       <c r="F43" s="27"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="I43" s="50"/>
+      <c r="I43" s="83"/>
       <c r="J43" s="26" t="s">
         <v>49</v>
       </c>
@@ -3735,17 +3702,17 @@
       <c r="O43" s="11"/>
       <c r="P43" s="11"/>
       <c r="Q43" s="11"/>
-      <c r="R43" s="51" t="s">
+      <c r="R43" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="S43" s="51"/>
-      <c r="T43" s="51"/>
-      <c r="U43" s="51"/>
-      <c r="V43" s="51"/>
-      <c r="W43" s="51"/>
-      <c r="X43" s="51"/>
-      <c r="Y43" s="51"/>
-      <c r="Z43" s="52"/>
+      <c r="S43" s="84"/>
+      <c r="T43" s="84"/>
+      <c r="U43" s="84"/>
+      <c r="V43" s="84"/>
+      <c r="W43" s="84"/>
+      <c r="X43" s="84"/>
+      <c r="Y43" s="84"/>
+      <c r="Z43" s="85"/>
       <c r="AB43" s="15"/>
       <c r="AC43" s="15"/>
       <c r="AD43" s="29"/>
@@ -3769,35 +3736,35 @@
       <c r="AZ43" s="8"/>
     </row>
     <row r="44" spans="2:52" ht="15" customHeight="1">
-      <c r="B44" s="53" t="s">
+      <c r="B44" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="55"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="57" t="s">
+      <c r="C44" s="87"/>
+      <c r="D44" s="87"/>
+      <c r="E44" s="87"/>
+      <c r="F44" s="87"/>
+      <c r="G44" s="79"/>
+      <c r="H44" s="79"/>
+      <c r="I44" s="79"/>
+      <c r="J44" s="79"/>
+      <c r="K44" s="79"/>
+      <c r="L44" s="79"/>
+      <c r="M44" s="88"/>
+      <c r="N44" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="O44" s="58"/>
-      <c r="P44" s="58"/>
-      <c r="Q44" s="58"/>
-      <c r="R44" s="58"/>
-      <c r="S44" s="58"/>
-      <c r="T44" s="58"/>
-      <c r="U44" s="58"/>
-      <c r="V44" s="58"/>
-      <c r="W44" s="58"/>
-      <c r="X44" s="58"/>
-      <c r="Y44" s="58"/>
-      <c r="Z44" s="59"/>
+      <c r="O44" s="90"/>
+      <c r="P44" s="90"/>
+      <c r="Q44" s="90"/>
+      <c r="R44" s="90"/>
+      <c r="S44" s="90"/>
+      <c r="T44" s="90"/>
+      <c r="U44" s="90"/>
+      <c r="V44" s="90"/>
+      <c r="W44" s="90"/>
+      <c r="X44" s="90"/>
+      <c r="Y44" s="90"/>
+      <c r="Z44" s="91"/>
       <c r="AB44" s="24"/>
       <c r="AC44" s="24"/>
       <c r="AD44" s="24"/>
@@ -3825,20 +3792,20 @@
       <c r="AZ44" s="3"/>
     </row>
     <row r="45" spans="2:52" ht="18" customHeight="1">
-      <c r="B45" s="60" t="s">
+      <c r="B45" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="61"/>
-      <c r="K45" s="61"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="62"/>
+      <c r="C45" s="93"/>
+      <c r="D45" s="93"/>
+      <c r="E45" s="93"/>
+      <c r="F45" s="93"/>
+      <c r="G45" s="93"/>
+      <c r="H45" s="93"/>
+      <c r="I45" s="93"/>
+      <c r="J45" s="93"/>
+      <c r="K45" s="93"/>
+      <c r="L45" s="93"/>
+      <c r="M45" s="94"/>
       <c r="N45" s="31">
         <v>1</v>
       </c>
@@ -3848,10 +3815,10 @@
       <c r="P45" s="31">
         <v>3</v>
       </c>
-      <c r="Q45" s="66" t="s">
+      <c r="Q45" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="R45" s="67"/>
+      <c r="R45" s="99"/>
       <c r="S45" s="31">
         <v>1</v>
       </c>
@@ -3903,18 +3870,18 @@
       <c r="AZ45" s="33"/>
     </row>
     <row r="46" spans="2:52" ht="18" customHeight="1">
-      <c r="B46" s="63"/>
-      <c r="C46" s="64"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="64"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="64"/>
-      <c r="J46" s="64"/>
-      <c r="K46" s="64"/>
-      <c r="L46" s="64"/>
-      <c r="M46" s="65"/>
+      <c r="B46" s="95"/>
+      <c r="C46" s="96"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="96"/>
+      <c r="H46" s="96"/>
+      <c r="I46" s="96"/>
+      <c r="J46" s="96"/>
+      <c r="K46" s="96"/>
+      <c r="L46" s="96"/>
+      <c r="M46" s="97"/>
       <c r="N46" s="31">
         <v>1</v>
       </c>
@@ -3924,10 +3891,10 @@
       <c r="P46" s="31">
         <v>3</v>
       </c>
-      <c r="Q46" s="66" t="s">
+      <c r="Q46" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="R46" s="67"/>
+      <c r="R46" s="99"/>
       <c r="S46" s="31">
         <v>1</v>
       </c>
@@ -3971,22 +3938,22 @@
       <c r="AZ46" s="34"/>
     </row>
     <row r="47" spans="2:52" ht="18" customHeight="1">
-      <c r="B47" s="68" t="s">
+      <c r="B47" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="68"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="69" t="s">
+      <c r="C47" s="100"/>
+      <c r="D47" s="89"/>
+      <c r="E47" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="70"/>
-      <c r="J47" s="70"/>
-      <c r="K47" s="70"/>
-      <c r="L47" s="70"/>
-      <c r="M47" s="71"/>
+      <c r="F47" s="102"/>
+      <c r="G47" s="102"/>
+      <c r="H47" s="102"/>
+      <c r="I47" s="102"/>
+      <c r="J47" s="102"/>
+      <c r="K47" s="102"/>
+      <c r="L47" s="102"/>
+      <c r="M47" s="103"/>
       <c r="N47" s="31">
         <v>1</v>
       </c>
@@ -3996,10 +3963,10 @@
       <c r="P47" s="31">
         <v>3</v>
       </c>
-      <c r="Q47" s="75" t="s">
+      <c r="Q47" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="R47" s="75"/>
+      <c r="R47" s="107"/>
       <c r="S47" s="31">
         <v>1</v>
       </c>
@@ -4043,18 +4010,18 @@
       <c r="AZ47" s="34"/>
     </row>
     <row r="48" spans="2:52" ht="18" customHeight="1">
-      <c r="B48" s="68"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="72"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="73"/>
-      <c r="I48" s="73"/>
-      <c r="J48" s="73"/>
-      <c r="K48" s="73"/>
-      <c r="L48" s="73"/>
-      <c r="M48" s="74"/>
+      <c r="B48" s="100"/>
+      <c r="C48" s="100"/>
+      <c r="D48" s="89"/>
+      <c r="E48" s="104"/>
+      <c r="F48" s="105"/>
+      <c r="G48" s="105"/>
+      <c r="H48" s="105"/>
+      <c r="I48" s="105"/>
+      <c r="J48" s="105"/>
+      <c r="K48" s="105"/>
+      <c r="L48" s="105"/>
+      <c r="M48" s="106"/>
       <c r="N48" s="36">
         <v>1</v>
       </c>
@@ -4064,10 +4031,10 @@
       <c r="P48" s="36">
         <v>3</v>
       </c>
-      <c r="Q48" s="76" t="s">
+      <c r="Q48" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="R48" s="76"/>
+      <c r="R48" s="108"/>
       <c r="S48" s="36">
         <v>1</v>
       </c>
@@ -4111,33 +4078,33 @@
       <c r="AZ48" s="34"/>
     </row>
     <row r="49" spans="2:52" ht="15" customHeight="1">
-      <c r="B49" s="68"/>
-      <c r="C49" s="68"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="72"/>
-      <c r="F49" s="73"/>
-      <c r="G49" s="73"/>
-      <c r="H49" s="73"/>
-      <c r="I49" s="73"/>
-      <c r="J49" s="73"/>
-      <c r="K49" s="73"/>
-      <c r="L49" s="73"/>
-      <c r="M49" s="74"/>
-      <c r="N49" s="77" t="s">
+      <c r="B49" s="100"/>
+      <c r="C49" s="100"/>
+      <c r="D49" s="89"/>
+      <c r="E49" s="104"/>
+      <c r="F49" s="105"/>
+      <c r="G49" s="105"/>
+      <c r="H49" s="105"/>
+      <c r="I49" s="105"/>
+      <c r="J49" s="105"/>
+      <c r="K49" s="105"/>
+      <c r="L49" s="105"/>
+      <c r="M49" s="106"/>
+      <c r="N49" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="O49" s="78"/>
-      <c r="P49" s="78"/>
-      <c r="Q49" s="78"/>
-      <c r="R49" s="78"/>
-      <c r="S49" s="78"/>
-      <c r="T49" s="78"/>
-      <c r="U49" s="78"/>
-      <c r="V49" s="78"/>
-      <c r="W49" s="78"/>
-      <c r="X49" s="78"/>
-      <c r="Y49" s="78"/>
-      <c r="Z49" s="79"/>
+      <c r="O49" s="110"/>
+      <c r="P49" s="110"/>
+      <c r="Q49" s="110"/>
+      <c r="R49" s="110"/>
+      <c r="S49" s="110"/>
+      <c r="T49" s="110"/>
+      <c r="U49" s="110"/>
+      <c r="V49" s="110"/>
+      <c r="W49" s="110"/>
+      <c r="X49" s="110"/>
+      <c r="Y49" s="110"/>
+      <c r="Z49" s="111"/>
       <c r="AB49" s="3"/>
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
@@ -4165,18 +4132,18 @@
       <c r="AZ49" s="38"/>
     </row>
     <row r="50" spans="2:52">
-      <c r="B50" s="68"/>
-      <c r="C50" s="68"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="72"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="73"/>
-      <c r="H50" s="73"/>
-      <c r="I50" s="73"/>
-      <c r="J50" s="73"/>
-      <c r="K50" s="73"/>
-      <c r="L50" s="73"/>
-      <c r="M50" s="74"/>
+      <c r="B50" s="100"/>
+      <c r="C50" s="100"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="104"/>
+      <c r="F50" s="105"/>
+      <c r="G50" s="105"/>
+      <c r="H50" s="105"/>
+      <c r="I50" s="105"/>
+      <c r="J50" s="105"/>
+      <c r="K50" s="105"/>
+      <c r="L50" s="105"/>
+      <c r="M50" s="106"/>
       <c r="N50" s="39"/>
       <c r="O50" s="40"/>
       <c r="P50" s="40"/>
@@ -4223,18 +4190,18 @@
       <c r="AZ50" s="42"/>
     </row>
     <row r="51" spans="2:52" ht="15" customHeight="1">
-      <c r="B51" s="68"/>
-      <c r="C51" s="68"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="73"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="73"/>
-      <c r="I51" s="73"/>
-      <c r="J51" s="73"/>
-      <c r="K51" s="73"/>
-      <c r="L51" s="73"/>
-      <c r="M51" s="74"/>
+      <c r="B51" s="100"/>
+      <c r="C51" s="100"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="104"/>
+      <c r="F51" s="105"/>
+      <c r="G51" s="105"/>
+      <c r="H51" s="105"/>
+      <c r="I51" s="105"/>
+      <c r="J51" s="105"/>
+      <c r="K51" s="105"/>
+      <c r="L51" s="105"/>
+      <c r="M51" s="106"/>
       <c r="N51" s="39"/>
       <c r="O51" s="40"/>
       <c r="P51" s="40"/>
@@ -4245,11 +4212,11 @@
       <c r="U51" s="40"/>
       <c r="V51" s="40"/>
       <c r="W51" s="40"/>
-      <c r="X51" s="80" t="s">
+      <c r="X51" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="Y51" s="80"/>
-      <c r="Z51" s="80"/>
+      <c r="Y51" s="112"/>
+      <c r="Z51" s="112"/>
       <c r="AB51" s="3"/>
       <c r="AC51" s="3"/>
       <c r="AD51" s="3"/>
@@ -4277,32 +4244,32 @@
       <c r="AZ51" s="42"/>
     </row>
     <row r="52" spans="2:52" ht="15" customHeight="1">
-      <c r="B52" s="68"/>
-      <c r="C52" s="68"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="81"/>
-      <c r="F52" s="82"/>
-      <c r="G52" s="82"/>
-      <c r="H52" s="82"/>
+      <c r="B52" s="100"/>
+      <c r="C52" s="100"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="113"/>
+      <c r="F52" s="114"/>
+      <c r="G52" s="114"/>
+      <c r="H52" s="114"/>
       <c r="I52" s="119" t="s">
         <v>75</v>
       </c>
       <c r="J52" s="120"/>
-      <c r="K52" s="82"/>
-      <c r="L52" s="82"/>
+      <c r="K52" s="114"/>
+      <c r="L52" s="114"/>
       <c r="M52" s="44"/>
-      <c r="N52" s="85" t="s">
+      <c r="N52" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="O52" s="86"/>
-      <c r="P52" s="86"/>
-      <c r="Q52" s="86"/>
-      <c r="R52" s="86"/>
-      <c r="S52" s="86"/>
-      <c r="T52" s="86"/>
-      <c r="U52" s="86"/>
-      <c r="V52" s="86"/>
-      <c r="W52" s="86"/>
+      <c r="O52" s="118"/>
+      <c r="P52" s="118"/>
+      <c r="Q52" s="118"/>
+      <c r="R52" s="118"/>
+      <c r="S52" s="118"/>
+      <c r="T52" s="118"/>
+      <c r="U52" s="118"/>
+      <c r="V52" s="118"/>
+      <c r="W52" s="118"/>
       <c r="X52" s="45"/>
       <c r="Y52" s="45"/>
       <c r="Z52" s="46"/>
@@ -4334,312 +4301,312 @@
     </row>
     <row r="53" spans="2:52" ht="27.75" customHeight="1"/>
     <row r="54" spans="2:52" ht="15" customHeight="1">
-      <c r="H54" s="92" t="s">
+      <c r="H54" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="I54" s="92"/>
-      <c r="J54" s="92"/>
-      <c r="K54" s="92"/>
-      <c r="L54" s="92" t="s">
+      <c r="I54" s="49"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="49"/>
+      <c r="L54" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="M54" s="92"/>
-      <c r="N54" s="92"/>
-      <c r="O54" s="92"/>
-      <c r="P54" s="92"/>
-      <c r="Q54" s="92"/>
-      <c r="R54" s="92"/>
-      <c r="S54" s="92"/>
-      <c r="T54" s="92"/>
-      <c r="V54" s="92" t="s">
+      <c r="M54" s="49"/>
+      <c r="N54" s="49"/>
+      <c r="O54" s="49"/>
+      <c r="P54" s="49"/>
+      <c r="Q54" s="49"/>
+      <c r="R54" s="49"/>
+      <c r="S54" s="49"/>
+      <c r="T54" s="49"/>
+      <c r="V54" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="W54" s="92"/>
-      <c r="X54" s="92"/>
+      <c r="W54" s="49"/>
+      <c r="X54" s="49"/>
     </row>
     <row r="55" spans="2:52" ht="15" customHeight="1">
-      <c r="H55" s="92" t="s">
+      <c r="H55" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="I55" s="92"/>
-      <c r="J55" s="92"/>
-      <c r="K55" s="92"/>
-      <c r="L55" s="113" t="s">
+      <c r="I55" s="49"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="49"/>
+      <c r="L55" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="M55" s="113"/>
-      <c r="N55" s="113"/>
-      <c r="O55" s="113"/>
-      <c r="P55" s="113"/>
-      <c r="Q55" s="113"/>
-      <c r="R55" s="113"/>
-      <c r="S55" s="113"/>
-      <c r="T55" s="113"/>
-      <c r="U55" s="113"/>
+      <c r="M55" s="51"/>
+      <c r="N55" s="51"/>
+      <c r="O55" s="51"/>
+      <c r="P55" s="51"/>
+      <c r="Q55" s="51"/>
+      <c r="R55" s="51"/>
+      <c r="S55" s="51"/>
+      <c r="T55" s="51"/>
+      <c r="U55" s="51"/>
       <c r="V55" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="W55" s="115">
+      <c r="W55" s="53">
         <v>10090</v>
       </c>
-      <c r="X55" s="115"/>
+      <c r="X55" s="53"/>
     </row>
     <row r="56" spans="2:52" ht="15" customHeight="1">
-      <c r="H56" s="92" t="s">
+      <c r="H56" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="I56" s="92"/>
-      <c r="J56" s="92"/>
-      <c r="K56" s="92"/>
-      <c r="L56" s="113"/>
-      <c r="M56" s="113"/>
-      <c r="N56" s="113"/>
-      <c r="O56" s="113"/>
-      <c r="P56" s="113"/>
-      <c r="Q56" s="113"/>
-      <c r="R56" s="113"/>
-      <c r="S56" s="113"/>
-      <c r="T56" s="113"/>
-      <c r="U56" s="113"/>
+      <c r="I56" s="49"/>
+      <c r="J56" s="49"/>
+      <c r="K56" s="49"/>
+      <c r="L56" s="51"/>
+      <c r="M56" s="51"/>
+      <c r="N56" s="51"/>
+      <c r="O56" s="51"/>
+      <c r="P56" s="51"/>
+      <c r="Q56" s="51"/>
+      <c r="R56" s="51"/>
+      <c r="S56" s="51"/>
+      <c r="T56" s="51"/>
+      <c r="U56" s="51"/>
       <c r="V56" s="6"/>
       <c r="W56" s="6"/>
       <c r="X56" s="6"/>
     </row>
     <row r="57" spans="2:52" ht="15" customHeight="1">
-      <c r="H57" s="101" t="s">
+      <c r="H57" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I57" s="101"/>
-      <c r="J57" s="101"/>
-      <c r="K57" s="101"/>
-      <c r="L57" s="114"/>
-      <c r="M57" s="114"/>
-      <c r="N57" s="114"/>
-      <c r="O57" s="114"/>
-      <c r="P57" s="114"/>
-      <c r="Q57" s="114"/>
-      <c r="R57" s="114"/>
-      <c r="S57" s="114"/>
-      <c r="T57" s="114"/>
-      <c r="U57" s="114"/>
+      <c r="I57" s="50"/>
+      <c r="J57" s="50"/>
+      <c r="K57" s="50"/>
+      <c r="L57" s="52"/>
+      <c r="M57" s="52"/>
+      <c r="N57" s="52"/>
+      <c r="O57" s="52"/>
+      <c r="P57" s="52"/>
+      <c r="Q57" s="52"/>
+      <c r="R57" s="52"/>
+      <c r="S57" s="52"/>
+      <c r="T57" s="52"/>
+      <c r="U57" s="52"/>
     </row>
     <row r="58" spans="2:52" ht="15" customHeight="1">
-      <c r="B58" s="116" t="s">
+      <c r="B58" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="110"/>
-      <c r="D58" s="110"/>
-      <c r="E58" s="110" t="s">
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="110"/>
-      <c r="G58" s="110"/>
-      <c r="H58" s="110"/>
-      <c r="I58" s="110"/>
+      <c r="F58" s="55"/>
+      <c r="G58" s="55"/>
+      <c r="H58" s="55"/>
+      <c r="I58" s="55"/>
       <c r="J58" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K58" s="110" t="s">
+      <c r="K58" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="L58" s="110"/>
-      <c r="M58" s="110"/>
-      <c r="N58" s="110"/>
-      <c r="O58" s="110"/>
-      <c r="P58" s="110"/>
-      <c r="Q58" s="110"/>
-      <c r="R58" s="110"/>
-      <c r="S58" s="110"/>
-      <c r="T58" s="110"/>
+      <c r="L58" s="55"/>
+      <c r="M58" s="55"/>
+      <c r="N58" s="55"/>
+      <c r="O58" s="55"/>
+      <c r="P58" s="55"/>
+      <c r="Q58" s="55"/>
+      <c r="R58" s="55"/>
+      <c r="S58" s="55"/>
+      <c r="T58" s="55"/>
       <c r="U58" s="7"/>
-      <c r="V58" s="111" t="s">
+      <c r="V58" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="W58" s="111"/>
-      <c r="X58" s="117" t="s">
+      <c r="W58" s="56"/>
+      <c r="X58" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="Y58" s="117"/>
-      <c r="Z58" s="118"/>
+      <c r="Y58" s="57"/>
+      <c r="Z58" s="58"/>
     </row>
     <row r="59" spans="2:52" ht="18.75" customHeight="1">
-      <c r="B59" s="98" t="s">
+      <c r="B59" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="89"/>
+      <c r="C59" s="60"/>
       <c r="D59" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H59" s="92" t="s">
+      <c r="H59" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="I59" s="92"/>
+      <c r="I59" s="49"/>
       <c r="J59" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K59" s="99" t="s">
+      <c r="K59" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="L59" s="99"/>
-      <c r="M59" s="99"/>
-      <c r="N59" s="100"/>
-      <c r="O59" s="100"/>
-      <c r="P59" s="100"/>
-      <c r="Q59" s="100"/>
-      <c r="R59" s="100"/>
-      <c r="S59" s="100"/>
-      <c r="T59" s="100"/>
+      <c r="L59" s="61"/>
+      <c r="M59" s="61"/>
+      <c r="N59" s="62"/>
+      <c r="O59" s="62"/>
+      <c r="P59" s="62"/>
+      <c r="Q59" s="62"/>
+      <c r="R59" s="62"/>
+      <c r="S59" s="62"/>
+      <c r="T59" s="62"/>
       <c r="U59" s="11"/>
-      <c r="V59" s="101" t="s">
+      <c r="V59" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="W59" s="101"/>
-      <c r="X59" s="102" t="s">
+      <c r="W59" s="50"/>
+      <c r="X59" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="Y59" s="102"/>
-      <c r="Z59" s="103"/>
+      <c r="Y59" s="63"/>
+      <c r="Z59" s="64"/>
     </row>
     <row r="60" spans="2:52" ht="15" customHeight="1">
-      <c r="B60" s="104" t="s">
+      <c r="B60" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C60" s="105"/>
-      <c r="D60" s="105"/>
-      <c r="E60" s="105"/>
-      <c r="F60" s="105"/>
-      <c r="G60" s="106"/>
-      <c r="H60" s="104" t="s">
+      <c r="C60" s="66"/>
+      <c r="D60" s="66"/>
+      <c r="E60" s="66"/>
+      <c r="F60" s="66"/>
+      <c r="G60" s="67"/>
+      <c r="H60" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="I60" s="105"/>
-      <c r="J60" s="105"/>
-      <c r="K60" s="105"/>
-      <c r="L60" s="105"/>
-      <c r="M60" s="106"/>
-      <c r="N60" s="110" t="s">
+      <c r="I60" s="66"/>
+      <c r="J60" s="66"/>
+      <c r="K60" s="66"/>
+      <c r="L60" s="66"/>
+      <c r="M60" s="67"/>
+      <c r="N60" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="O60" s="110"/>
-      <c r="P60" s="110"/>
-      <c r="Q60" s="110"/>
-      <c r="R60" s="111" t="s">
+      <c r="O60" s="55"/>
+      <c r="P60" s="55"/>
+      <c r="Q60" s="55"/>
+      <c r="R60" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="S60" s="111"/>
-      <c r="T60" s="111"/>
-      <c r="U60" s="111"/>
-      <c r="V60" s="111"/>
-      <c r="W60" s="111"/>
-      <c r="X60" s="111"/>
-      <c r="Y60" s="111"/>
-      <c r="Z60" s="112"/>
+      <c r="S60" s="56"/>
+      <c r="T60" s="56"/>
+      <c r="U60" s="56"/>
+      <c r="V60" s="56"/>
+      <c r="W60" s="56"/>
+      <c r="X60" s="56"/>
+      <c r="Y60" s="56"/>
+      <c r="Z60" s="71"/>
     </row>
     <row r="61" spans="2:52" ht="15" customHeight="1">
-      <c r="B61" s="107"/>
-      <c r="C61" s="108"/>
-      <c r="D61" s="108"/>
-      <c r="E61" s="108"/>
-      <c r="F61" s="108"/>
-      <c r="G61" s="109"/>
-      <c r="H61" s="107"/>
-      <c r="I61" s="108"/>
-      <c r="J61" s="108"/>
-      <c r="K61" s="108"/>
-      <c r="L61" s="108"/>
-      <c r="M61" s="109"/>
-      <c r="N61" s="89"/>
-      <c r="O61" s="89"/>
-      <c r="P61" s="89"/>
-      <c r="Q61" s="89"/>
-      <c r="R61" s="92"/>
-      <c r="S61" s="92"/>
-      <c r="T61" s="92"/>
-      <c r="U61" s="92"/>
+      <c r="B61" s="68"/>
+      <c r="C61" s="69"/>
+      <c r="D61" s="69"/>
+      <c r="E61" s="69"/>
+      <c r="F61" s="69"/>
+      <c r="G61" s="70"/>
+      <c r="H61" s="68"/>
+      <c r="I61" s="69"/>
+      <c r="J61" s="69"/>
+      <c r="K61" s="69"/>
+      <c r="L61" s="69"/>
+      <c r="M61" s="70"/>
+      <c r="N61" s="60"/>
+      <c r="O61" s="60"/>
+      <c r="P61" s="60"/>
+      <c r="Q61" s="60"/>
+      <c r="R61" s="123"/>
+      <c r="S61" s="123"/>
+      <c r="T61" s="123"/>
+      <c r="U61" s="123"/>
       <c r="V61" s="8" t="s">
         <v>26</v>
       </c>
       <c r="W61" s="8"/>
-      <c r="X61" s="96" t="s">
+      <c r="X61" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="Y61" s="96"/>
-      <c r="Z61" s="97"/>
+      <c r="Y61" s="72"/>
+      <c r="Z61" s="73"/>
     </row>
     <row r="62" spans="2:52" ht="15" customHeight="1">
-      <c r="B62" s="87" t="s">
+      <c r="B62" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="88"/>
-      <c r="D62" s="88"/>
-      <c r="E62" s="88"/>
-      <c r="F62" s="88"/>
-      <c r="G62" s="95"/>
-      <c r="H62" s="87" t="s">
+      <c r="C62" s="75"/>
+      <c r="D62" s="75"/>
+      <c r="E62" s="75"/>
+      <c r="F62" s="75"/>
+      <c r="G62" s="76"/>
+      <c r="H62" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="I62" s="88"/>
-      <c r="J62" s="88"/>
-      <c r="K62" s="88"/>
-      <c r="L62" s="88"/>
-      <c r="M62" s="95"/>
-      <c r="N62" s="89"/>
-      <c r="O62" s="89"/>
-      <c r="P62" s="89"/>
-      <c r="Q62" s="89"/>
-      <c r="R62" s="92"/>
-      <c r="S62" s="92"/>
-      <c r="T62" s="92"/>
-      <c r="U62" s="92"/>
+      <c r="I62" s="75"/>
+      <c r="J62" s="75"/>
+      <c r="K62" s="75"/>
+      <c r="L62" s="75"/>
+      <c r="M62" s="76"/>
+      <c r="N62" s="60"/>
+      <c r="O62" s="60"/>
+      <c r="P62" s="60"/>
+      <c r="Q62" s="60"/>
+      <c r="R62" s="49"/>
+      <c r="S62" s="49"/>
+      <c r="T62" s="49"/>
+      <c r="U62" s="49"/>
       <c r="V62" s="8" t="s">
         <v>29</v>
       </c>
       <c r="W62" s="8"/>
-      <c r="X62" s="96" t="s">
+      <c r="X62" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="Y62" s="96"/>
-      <c r="Z62" s="97"/>
+      <c r="Y62" s="72"/>
+      <c r="Z62" s="73"/>
     </row>
     <row r="63" spans="2:52" ht="15" customHeight="1">
-      <c r="B63" s="87"/>
-      <c r="C63" s="88"/>
-      <c r="D63" s="88"/>
-      <c r="E63" s="88"/>
-      <c r="F63" s="88"/>
-      <c r="G63" s="95"/>
-      <c r="H63" s="87"/>
-      <c r="I63" s="88"/>
-      <c r="J63" s="88"/>
-      <c r="K63" s="88"/>
-      <c r="L63" s="88"/>
-      <c r="M63" s="95"/>
-      <c r="N63" s="89"/>
-      <c r="O63" s="89"/>
-      <c r="P63" s="89"/>
-      <c r="Q63" s="89"/>
-      <c r="R63" s="90"/>
-      <c r="S63" s="90"/>
-      <c r="T63" s="90"/>
-      <c r="U63" s="90"/>
+      <c r="B63" s="74"/>
+      <c r="C63" s="75"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="75"/>
+      <c r="F63" s="75"/>
+      <c r="G63" s="76"/>
+      <c r="H63" s="74"/>
+      <c r="I63" s="75"/>
+      <c r="J63" s="75"/>
+      <c r="K63" s="75"/>
+      <c r="L63" s="75"/>
+      <c r="M63" s="76"/>
+      <c r="N63" s="60"/>
+      <c r="O63" s="60"/>
+      <c r="P63" s="60"/>
+      <c r="Q63" s="60"/>
+      <c r="R63" s="77"/>
+      <c r="S63" s="77"/>
+      <c r="T63" s="77"/>
+      <c r="U63" s="77"/>
       <c r="V63" s="8" t="s">
         <v>30</v>
       </c>
       <c r="W63" s="8"/>
-      <c r="X63" s="96" t="s">
+      <c r="X63" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="Y63" s="96"/>
-      <c r="Z63" s="97"/>
+      <c r="Y63" s="72"/>
+      <c r="Z63" s="73"/>
     </row>
     <row r="64" spans="2:52" ht="15" customHeight="1">
-      <c r="B64" s="87" t="s">
+      <c r="B64" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="88"/>
+      <c r="C64" s="75"/>
       <c r="D64" s="15">
         <v>3022053929</v>
       </c>
@@ -4652,10 +4619,10 @@
       <c r="G64" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H64" s="87" t="s">
+      <c r="H64" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I64" s="88"/>
+      <c r="I64" s="75"/>
       <c r="J64" s="15">
         <v>3022053929</v>
       </c>
@@ -4668,70 +4635,70 @@
       <c r="M64" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="N64" s="89" t="s">
+      <c r="N64" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="O64" s="89"/>
-      <c r="P64" s="89"/>
-      <c r="Q64" s="89"/>
-      <c r="R64" s="96" t="s">
+      <c r="O64" s="60"/>
+      <c r="P64" s="60"/>
+      <c r="Q64" s="60"/>
+      <c r="R64" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="S64" s="96"/>
-      <c r="T64" s="96"/>
-      <c r="U64" s="96"/>
+      <c r="S64" s="72"/>
+      <c r="T64" s="72"/>
+      <c r="U64" s="72"/>
       <c r="V64" s="8" t="s">
         <v>35</v>
       </c>
       <c r="W64" s="8"/>
-      <c r="X64" s="90" t="s">
+      <c r="X64" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y64" s="90"/>
-      <c r="Z64" s="91"/>
+      <c r="Y64" s="77"/>
+      <c r="Z64" s="78"/>
     </row>
     <row r="65" spans="2:26" ht="15" customHeight="1">
-      <c r="B65" s="87" t="s">
+      <c r="B65" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C65" s="88"/>
-      <c r="D65" s="88" t="s">
+      <c r="C65" s="75"/>
+      <c r="D65" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="E65" s="88"/>
-      <c r="F65" s="88"/>
+      <c r="E65" s="75"/>
+      <c r="F65" s="75"/>
       <c r="G65" s="22"/>
-      <c r="H65" s="87" t="s">
+      <c r="H65" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="I65" s="88"/>
-      <c r="J65" s="88" t="s">
+      <c r="I65" s="75"/>
+      <c r="J65" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="K65" s="88"/>
-      <c r="L65" s="88"/>
+      <c r="K65" s="75"/>
+      <c r="L65" s="75"/>
       <c r="M65" s="22"/>
-      <c r="N65" s="89" t="s">
+      <c r="N65" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="O65" s="89"/>
-      <c r="P65" s="89"/>
-      <c r="Q65" s="89"/>
-      <c r="R65" s="90" t="s">
+      <c r="O65" s="60"/>
+      <c r="P65" s="60"/>
+      <c r="Q65" s="60"/>
+      <c r="R65" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="S65" s="90"/>
-      <c r="T65" s="90"/>
-      <c r="U65" s="90"/>
+      <c r="S65" s="77"/>
+      <c r="T65" s="77"/>
+      <c r="U65" s="77"/>
       <c r="V65" s="8" t="s">
         <v>40</v>
       </c>
       <c r="W65" s="8"/>
-      <c r="X65" s="90" t="s">
+      <c r="X65" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y65" s="90"/>
-      <c r="Z65" s="91"/>
+      <c r="Y65" s="77"/>
+      <c r="Z65" s="78"/>
     </row>
     <row r="66" spans="2:26" ht="15" customHeight="1">
       <c r="B66" s="23"/>
@@ -4746,70 +4713,70 @@
       <c r="K66" s="17"/>
       <c r="L66" s="17"/>
       <c r="M66" s="22"/>
-      <c r="N66" s="89" t="s">
+      <c r="N66" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="O66" s="89"/>
-      <c r="P66" s="89"/>
-      <c r="Q66" s="89"/>
-      <c r="R66" s="90" t="s">
+      <c r="O66" s="60"/>
+      <c r="P66" s="60"/>
+      <c r="Q66" s="60"/>
+      <c r="R66" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="S66" s="90"/>
-      <c r="T66" s="90"/>
-      <c r="U66" s="90"/>
+      <c r="S66" s="77"/>
+      <c r="T66" s="77"/>
+      <c r="U66" s="77"/>
       <c r="V66" s="8" t="s">
         <v>42</v>
       </c>
       <c r="W66" s="8"/>
-      <c r="X66" s="90" t="s">
+      <c r="X66" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y66" s="90"/>
-      <c r="Z66" s="91"/>
+      <c r="Y66" s="77"/>
+      <c r="Z66" s="78"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1">
-      <c r="B67" s="87" t="s">
+      <c r="B67" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="C67" s="88"/>
-      <c r="D67" s="88" t="s">
+      <c r="C67" s="75"/>
+      <c r="D67" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="E67" s="88"/>
-      <c r="F67" s="88"/>
+      <c r="E67" s="75"/>
+      <c r="F67" s="75"/>
       <c r="G67" s="22"/>
-      <c r="H67" s="87" t="s">
+      <c r="H67" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="I67" s="88"/>
-      <c r="J67" s="88" t="s">
+      <c r="I67" s="75"/>
+      <c r="J67" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="K67" s="88"/>
-      <c r="L67" s="88"/>
+      <c r="K67" s="75"/>
+      <c r="L67" s="75"/>
       <c r="M67" s="22"/>
-      <c r="N67" s="89" t="s">
+      <c r="N67" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="O67" s="89"/>
-      <c r="P67" s="89"/>
-      <c r="Q67" s="89"/>
-      <c r="R67" s="90">
+      <c r="O67" s="60"/>
+      <c r="P67" s="60"/>
+      <c r="Q67" s="60"/>
+      <c r="R67" s="77">
         <v>0</v>
       </c>
-      <c r="S67" s="90"/>
-      <c r="T67" s="90"/>
-      <c r="U67" s="90"/>
+      <c r="S67" s="77"/>
+      <c r="T67" s="77"/>
+      <c r="U67" s="77"/>
       <c r="V67" s="8" t="s">
         <v>46</v>
       </c>
       <c r="W67" s="8"/>
-      <c r="X67" s="90" t="s">
+      <c r="X67" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="Y67" s="90"/>
-      <c r="Z67" s="91"/>
+      <c r="Y67" s="77"/>
+      <c r="Z67" s="78"/>
     </row>
     <row r="68" spans="2:26" ht="15" customHeight="1">
       <c r="B68" s="23"/>
@@ -4824,39 +4791,39 @@
       <c r="K68" s="17"/>
       <c r="L68" s="17"/>
       <c r="M68" s="22"/>
-      <c r="N68" s="89"/>
-      <c r="O68" s="89"/>
-      <c r="P68" s="89"/>
-      <c r="Q68" s="89"/>
-      <c r="R68" s="92"/>
-      <c r="S68" s="92"/>
-      <c r="T68" s="92"/>
-      <c r="U68" s="92"/>
-      <c r="V68" s="55" t="s">
+      <c r="N68" s="60"/>
+      <c r="O68" s="60"/>
+      <c r="P68" s="60"/>
+      <c r="Q68" s="60"/>
+      <c r="R68" s="49"/>
+      <c r="S68" s="49"/>
+      <c r="T68" s="49"/>
+      <c r="U68" s="49"/>
+      <c r="V68" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="W68" s="55"/>
-      <c r="X68" s="93" t="s">
+      <c r="W68" s="79"/>
+      <c r="X68" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="Y68" s="93"/>
-      <c r="Z68" s="94"/>
+      <c r="Y68" s="80"/>
+      <c r="Z68" s="81"/>
     </row>
     <row r="69" spans="2:26" ht="15" customHeight="1">
-      <c r="B69" s="49" t="s">
+      <c r="B69" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="C69" s="50"/>
+      <c r="C69" s="83"/>
       <c r="D69" s="26" t="s">
         <v>49</v>
       </c>
       <c r="E69" s="27"/>
       <c r="F69" s="27"/>
       <c r="G69" s="28"/>
-      <c r="H69" s="49" t="s">
+      <c r="H69" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="I69" s="50"/>
+      <c r="I69" s="83"/>
       <c r="J69" s="26" t="s">
         <v>49</v>
       </c>
@@ -4869,64 +4836,64 @@
       <c r="O69" s="11"/>
       <c r="P69" s="11"/>
       <c r="Q69" s="11"/>
-      <c r="R69" s="51" t="s">
+      <c r="R69" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="S69" s="51"/>
-      <c r="T69" s="51"/>
-      <c r="U69" s="51"/>
-      <c r="V69" s="51"/>
-      <c r="W69" s="51"/>
-      <c r="X69" s="51"/>
-      <c r="Y69" s="51"/>
-      <c r="Z69" s="52"/>
+      <c r="S69" s="84"/>
+      <c r="T69" s="84"/>
+      <c r="U69" s="84"/>
+      <c r="V69" s="84"/>
+      <c r="W69" s="84"/>
+      <c r="X69" s="84"/>
+      <c r="Y69" s="84"/>
+      <c r="Z69" s="85"/>
     </row>
     <row r="70" spans="2:26" ht="15" customHeight="1">
-      <c r="B70" s="53" t="s">
+      <c r="B70" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="C70" s="54"/>
-      <c r="D70" s="54"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="54"/>
-      <c r="G70" s="55"/>
-      <c r="H70" s="55"/>
-      <c r="I70" s="55"/>
-      <c r="J70" s="55"/>
-      <c r="K70" s="55"/>
-      <c r="L70" s="55"/>
-      <c r="M70" s="56"/>
-      <c r="N70" s="57" t="s">
+      <c r="C70" s="87"/>
+      <c r="D70" s="87"/>
+      <c r="E70" s="87"/>
+      <c r="F70" s="87"/>
+      <c r="G70" s="79"/>
+      <c r="H70" s="79"/>
+      <c r="I70" s="79"/>
+      <c r="J70" s="79"/>
+      <c r="K70" s="79"/>
+      <c r="L70" s="79"/>
+      <c r="M70" s="88"/>
+      <c r="N70" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="O70" s="58"/>
-      <c r="P70" s="58"/>
-      <c r="Q70" s="58"/>
-      <c r="R70" s="58"/>
-      <c r="S70" s="58"/>
-      <c r="T70" s="58"/>
-      <c r="U70" s="58"/>
-      <c r="V70" s="58"/>
-      <c r="W70" s="58"/>
-      <c r="X70" s="58"/>
-      <c r="Y70" s="58"/>
-      <c r="Z70" s="59"/>
+      <c r="O70" s="90"/>
+      <c r="P70" s="90"/>
+      <c r="Q70" s="90"/>
+      <c r="R70" s="90"/>
+      <c r="S70" s="90"/>
+      <c r="T70" s="90"/>
+      <c r="U70" s="90"/>
+      <c r="V70" s="90"/>
+      <c r="W70" s="90"/>
+      <c r="X70" s="90"/>
+      <c r="Y70" s="90"/>
+      <c r="Z70" s="91"/>
     </row>
     <row r="71" spans="2:26" ht="18" customHeight="1">
-      <c r="B71" s="60" t="s">
+      <c r="B71" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="C71" s="61"/>
-      <c r="D71" s="61"/>
-      <c r="E71" s="61"/>
-      <c r="F71" s="61"/>
-      <c r="G71" s="61"/>
-      <c r="H71" s="61"/>
-      <c r="I71" s="61"/>
-      <c r="J71" s="61"/>
-      <c r="K71" s="61"/>
-      <c r="L71" s="61"/>
-      <c r="M71" s="62"/>
+      <c r="C71" s="93"/>
+      <c r="D71" s="93"/>
+      <c r="E71" s="93"/>
+      <c r="F71" s="93"/>
+      <c r="G71" s="93"/>
+      <c r="H71" s="93"/>
+      <c r="I71" s="93"/>
+      <c r="J71" s="93"/>
+      <c r="K71" s="93"/>
+      <c r="L71" s="93"/>
+      <c r="M71" s="94"/>
       <c r="N71" s="31">
         <v>1</v>
       </c>
@@ -4936,10 +4903,10 @@
       <c r="P71" s="31">
         <v>3</v>
       </c>
-      <c r="Q71" s="66" t="s">
+      <c r="Q71" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="R71" s="67"/>
+      <c r="R71" s="99"/>
       <c r="S71" s="31">
         <v>1</v>
       </c>
@@ -4966,18 +4933,18 @@
       </c>
     </row>
     <row r="72" spans="2:26" ht="18" customHeight="1">
-      <c r="B72" s="63"/>
-      <c r="C72" s="64"/>
-      <c r="D72" s="64"/>
-      <c r="E72" s="64"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="64"/>
-      <c r="H72" s="64"/>
-      <c r="I72" s="64"/>
-      <c r="J72" s="64"/>
-      <c r="K72" s="64"/>
-      <c r="L72" s="64"/>
-      <c r="M72" s="65"/>
+      <c r="B72" s="95"/>
+      <c r="C72" s="96"/>
+      <c r="D72" s="96"/>
+      <c r="E72" s="96"/>
+      <c r="F72" s="96"/>
+      <c r="G72" s="96"/>
+      <c r="H72" s="96"/>
+      <c r="I72" s="96"/>
+      <c r="J72" s="96"/>
+      <c r="K72" s="96"/>
+      <c r="L72" s="96"/>
+      <c r="M72" s="97"/>
       <c r="N72" s="31">
         <v>1</v>
       </c>
@@ -4987,10 +4954,10 @@
       <c r="P72" s="31">
         <v>3</v>
       </c>
-      <c r="Q72" s="66" t="s">
+      <c r="Q72" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="R72" s="67"/>
+      <c r="R72" s="99"/>
       <c r="S72" s="31">
         <v>1</v>
       </c>
@@ -5009,22 +4976,22 @@
       <c r="Z72" s="32"/>
     </row>
     <row r="73" spans="2:26" ht="18" customHeight="1">
-      <c r="B73" s="68" t="s">
+      <c r="B73" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="C73" s="68"/>
-      <c r="D73" s="57"/>
-      <c r="E73" s="69" t="s">
+      <c r="C73" s="100"/>
+      <c r="D73" s="89"/>
+      <c r="E73" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="F73" s="70"/>
-      <c r="G73" s="70"/>
-      <c r="H73" s="70"/>
-      <c r="I73" s="70"/>
-      <c r="J73" s="70"/>
-      <c r="K73" s="70"/>
-      <c r="L73" s="70"/>
-      <c r="M73" s="71"/>
+      <c r="F73" s="102"/>
+      <c r="G73" s="102"/>
+      <c r="H73" s="102"/>
+      <c r="I73" s="102"/>
+      <c r="J73" s="102"/>
+      <c r="K73" s="102"/>
+      <c r="L73" s="102"/>
+      <c r="M73" s="103"/>
       <c r="N73" s="31">
         <v>1</v>
       </c>
@@ -5034,10 +5001,10 @@
       <c r="P73" s="31">
         <v>3</v>
       </c>
-      <c r="Q73" s="75" t="s">
+      <c r="Q73" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="R73" s="75"/>
+      <c r="R73" s="107"/>
       <c r="S73" s="31">
         <v>1</v>
       </c>
@@ -5056,18 +5023,18 @@
       <c r="Z73" s="32"/>
     </row>
     <row r="74" spans="2:26" ht="18" customHeight="1">
-      <c r="B74" s="68"/>
-      <c r="C74" s="68"/>
-      <c r="D74" s="57"/>
-      <c r="E74" s="72"/>
-      <c r="F74" s="73"/>
-      <c r="G74" s="73"/>
-      <c r="H74" s="73"/>
-      <c r="I74" s="73"/>
-      <c r="J74" s="73"/>
-      <c r="K74" s="73"/>
-      <c r="L74" s="73"/>
-      <c r="M74" s="74"/>
+      <c r="B74" s="100"/>
+      <c r="C74" s="100"/>
+      <c r="D74" s="89"/>
+      <c r="E74" s="104"/>
+      <c r="F74" s="105"/>
+      <c r="G74" s="105"/>
+      <c r="H74" s="105"/>
+      <c r="I74" s="105"/>
+      <c r="J74" s="105"/>
+      <c r="K74" s="105"/>
+      <c r="L74" s="105"/>
+      <c r="M74" s="106"/>
       <c r="N74" s="36">
         <v>1</v>
       </c>
@@ -5077,10 +5044,10 @@
       <c r="P74" s="36">
         <v>3</v>
       </c>
-      <c r="Q74" s="76" t="s">
+      <c r="Q74" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="R74" s="76"/>
+      <c r="R74" s="108"/>
       <c r="S74" s="36">
         <v>1</v>
       </c>
@@ -5099,47 +5066,47 @@
       <c r="Z74" s="37"/>
     </row>
     <row r="75" spans="2:26" ht="15" customHeight="1">
-      <c r="B75" s="68"/>
-      <c r="C75" s="68"/>
-      <c r="D75" s="57"/>
-      <c r="E75" s="72"/>
-      <c r="F75" s="73"/>
-      <c r="G75" s="73"/>
-      <c r="H75" s="73"/>
-      <c r="I75" s="73"/>
-      <c r="J75" s="73"/>
-      <c r="K75" s="73"/>
-      <c r="L75" s="73"/>
-      <c r="M75" s="74"/>
-      <c r="N75" s="77" t="s">
+      <c r="B75" s="100"/>
+      <c r="C75" s="100"/>
+      <c r="D75" s="89"/>
+      <c r="E75" s="104"/>
+      <c r="F75" s="105"/>
+      <c r="G75" s="105"/>
+      <c r="H75" s="105"/>
+      <c r="I75" s="105"/>
+      <c r="J75" s="105"/>
+      <c r="K75" s="105"/>
+      <c r="L75" s="105"/>
+      <c r="M75" s="106"/>
+      <c r="N75" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="O75" s="78"/>
-      <c r="P75" s="78"/>
-      <c r="Q75" s="78"/>
-      <c r="R75" s="78"/>
-      <c r="S75" s="78"/>
-      <c r="T75" s="78"/>
-      <c r="U75" s="78"/>
-      <c r="V75" s="78"/>
-      <c r="W75" s="78"/>
-      <c r="X75" s="78"/>
-      <c r="Y75" s="78"/>
-      <c r="Z75" s="79"/>
+      <c r="O75" s="110"/>
+      <c r="P75" s="110"/>
+      <c r="Q75" s="110"/>
+      <c r="R75" s="110"/>
+      <c r="S75" s="110"/>
+      <c r="T75" s="110"/>
+      <c r="U75" s="110"/>
+      <c r="V75" s="110"/>
+      <c r="W75" s="110"/>
+      <c r="X75" s="110"/>
+      <c r="Y75" s="110"/>
+      <c r="Z75" s="111"/>
     </row>
     <row r="76" spans="2:26">
-      <c r="B76" s="68"/>
-      <c r="C76" s="68"/>
-      <c r="D76" s="57"/>
-      <c r="E76" s="72"/>
-      <c r="F76" s="73"/>
-      <c r="G76" s="73"/>
-      <c r="H76" s="73"/>
-      <c r="I76" s="73"/>
-      <c r="J76" s="73"/>
-      <c r="K76" s="73"/>
-      <c r="L76" s="73"/>
-      <c r="M76" s="74"/>
+      <c r="B76" s="100"/>
+      <c r="C76" s="100"/>
+      <c r="D76" s="89"/>
+      <c r="E76" s="104"/>
+      <c r="F76" s="105"/>
+      <c r="G76" s="105"/>
+      <c r="H76" s="105"/>
+      <c r="I76" s="105"/>
+      <c r="J76" s="105"/>
+      <c r="K76" s="105"/>
+      <c r="L76" s="105"/>
+      <c r="M76" s="106"/>
       <c r="N76" s="39"/>
       <c r="O76" s="40"/>
       <c r="P76" s="40"/>
@@ -5161,18 +5128,18 @@
       </c>
     </row>
     <row r="77" spans="2:26" ht="15" customHeight="1">
-      <c r="B77" s="68"/>
-      <c r="C77" s="68"/>
-      <c r="D77" s="57"/>
-      <c r="E77" s="72"/>
-      <c r="F77" s="73"/>
-      <c r="G77" s="73"/>
-      <c r="H77" s="73"/>
-      <c r="I77" s="73"/>
-      <c r="J77" s="73"/>
-      <c r="K77" s="73"/>
-      <c r="L77" s="73"/>
-      <c r="M77" s="74"/>
+      <c r="B77" s="100"/>
+      <c r="C77" s="100"/>
+      <c r="D77" s="89"/>
+      <c r="E77" s="104"/>
+      <c r="F77" s="105"/>
+      <c r="G77" s="105"/>
+      <c r="H77" s="105"/>
+      <c r="I77" s="105"/>
+      <c r="J77" s="105"/>
+      <c r="K77" s="105"/>
+      <c r="L77" s="105"/>
+      <c r="M77" s="106"/>
       <c r="N77" s="39"/>
       <c r="O77" s="40"/>
       <c r="P77" s="40"/>
@@ -5183,182 +5150,122 @@
       <c r="U77" s="40"/>
       <c r="V77" s="40"/>
       <c r="W77" s="40"/>
-      <c r="X77" s="80" t="s">
+      <c r="X77" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="Y77" s="80"/>
-      <c r="Z77" s="80"/>
+      <c r="Y77" s="112"/>
+      <c r="Z77" s="112"/>
     </row>
     <row r="78" spans="2:26" ht="15" customHeight="1">
-      <c r="B78" s="68"/>
-      <c r="C78" s="68"/>
-      <c r="D78" s="57"/>
-      <c r="E78" s="81"/>
-      <c r="F78" s="82"/>
-      <c r="G78" s="82"/>
-      <c r="H78" s="82"/>
-      <c r="I78" s="83" t="s">
+      <c r="B78" s="100"/>
+      <c r="C78" s="100"/>
+      <c r="D78" s="89"/>
+      <c r="E78" s="113"/>
+      <c r="F78" s="114"/>
+      <c r="G78" s="114"/>
+      <c r="H78" s="114"/>
+      <c r="I78" s="121" t="s">
         <v>77</v>
       </c>
-      <c r="J78" s="84"/>
-      <c r="K78" s="82"/>
-      <c r="L78" s="82"/>
+      <c r="J78" s="122"/>
+      <c r="K78" s="114"/>
+      <c r="L78" s="114"/>
       <c r="M78" s="44"/>
-      <c r="N78" s="85" t="s">
+      <c r="N78" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="O78" s="86"/>
-      <c r="P78" s="86"/>
-      <c r="Q78" s="86"/>
-      <c r="R78" s="86"/>
-      <c r="S78" s="86"/>
-      <c r="T78" s="86"/>
-      <c r="U78" s="86"/>
-      <c r="V78" s="86"/>
-      <c r="W78" s="86"/>
+      <c r="O78" s="118"/>
+      <c r="P78" s="118"/>
+      <c r="Q78" s="118"/>
+      <c r="R78" s="118"/>
+      <c r="S78" s="118"/>
+      <c r="T78" s="118"/>
+      <c r="U78" s="118"/>
+      <c r="V78" s="118"/>
+      <c r="W78" s="118"/>
       <c r="X78" s="45"/>
       <c r="Y78" s="45"/>
       <c r="Z78" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="232">
-    <mergeCell ref="B2:F5"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L2:T2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:U5"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="K6:T6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="K7:T7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="B8:G9"/>
-    <mergeCell ref="H8:M9"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="R8:Z8"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="B10:G11"/>
-    <mergeCell ref="H10:M11"/>
-    <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="R10:U10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="R11:U11"/>
-    <mergeCell ref="X11:Z11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="R12:U12"/>
-    <mergeCell ref="X12:Z12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="R13:U13"/>
-    <mergeCell ref="X13:Z13"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="R14:U14"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="R15:U15"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="R16:U16"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="X16:Z16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="R17:Z17"/>
-    <mergeCell ref="B18:M18"/>
-    <mergeCell ref="N18:Z18"/>
-    <mergeCell ref="B19:M20"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="B21:D26"/>
-    <mergeCell ref="E21:M25"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="N23:Z23"/>
-    <mergeCell ref="X25:Z25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="N26:W26"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="L28:T28"/>
-    <mergeCell ref="V28:X28"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="L29:U31"/>
-    <mergeCell ref="W29:X29"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="K32:T32"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="X32:Z32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="K33:T33"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="X33:Z33"/>
-    <mergeCell ref="B34:G35"/>
-    <mergeCell ref="H34:M35"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="R34:Z34"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="R35:U35"/>
-    <mergeCell ref="X35:Z35"/>
-    <mergeCell ref="B36:G37"/>
-    <mergeCell ref="H36:M37"/>
-    <mergeCell ref="N36:Q36"/>
-    <mergeCell ref="R36:U36"/>
-    <mergeCell ref="X36:Z36"/>
-    <mergeCell ref="N37:Q37"/>
-    <mergeCell ref="R37:U37"/>
-    <mergeCell ref="X37:Z37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="N38:Q38"/>
-    <mergeCell ref="R38:U38"/>
-    <mergeCell ref="X38:Z38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="N39:Q39"/>
-    <mergeCell ref="R39:U39"/>
-    <mergeCell ref="X39:Z39"/>
-    <mergeCell ref="N40:Q40"/>
-    <mergeCell ref="R40:U40"/>
-    <mergeCell ref="X40:Z40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="N41:Q41"/>
-    <mergeCell ref="R41:U41"/>
-    <mergeCell ref="X41:Z41"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R42:U42"/>
-    <mergeCell ref="V42:W42"/>
-    <mergeCell ref="X42:Z42"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="R69:Z69"/>
+    <mergeCell ref="B70:M70"/>
+    <mergeCell ref="N70:Z70"/>
+    <mergeCell ref="B71:M72"/>
+    <mergeCell ref="Q71:R71"/>
+    <mergeCell ref="Q72:R72"/>
+    <mergeCell ref="B73:D78"/>
+    <mergeCell ref="E73:M77"/>
+    <mergeCell ref="Q73:R73"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="N75:Z75"/>
+    <mergeCell ref="X77:Z77"/>
+    <mergeCell ref="E78:H78"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="K78:L78"/>
+    <mergeCell ref="N78:W78"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="J67:L67"/>
+    <mergeCell ref="N67:Q67"/>
+    <mergeCell ref="R67:U67"/>
+    <mergeCell ref="X67:Z67"/>
+    <mergeCell ref="N68:Q68"/>
+    <mergeCell ref="R68:U68"/>
+    <mergeCell ref="V68:W68"/>
+    <mergeCell ref="X68:Z68"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="J65:L65"/>
+    <mergeCell ref="N65:Q65"/>
+    <mergeCell ref="R65:U65"/>
+    <mergeCell ref="X65:Z65"/>
+    <mergeCell ref="N66:Q66"/>
+    <mergeCell ref="R66:U66"/>
+    <mergeCell ref="X66:Z66"/>
+    <mergeCell ref="B62:G63"/>
+    <mergeCell ref="H62:M63"/>
+    <mergeCell ref="N62:Q62"/>
+    <mergeCell ref="R62:U62"/>
+    <mergeCell ref="X62:Z62"/>
+    <mergeCell ref="N63:Q63"/>
+    <mergeCell ref="R63:U63"/>
+    <mergeCell ref="X63:Z63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="N64:Q64"/>
+    <mergeCell ref="R64:U64"/>
+    <mergeCell ref="X64:Z64"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="K59:T59"/>
+    <mergeCell ref="V59:W59"/>
+    <mergeCell ref="X59:Z59"/>
+    <mergeCell ref="B60:G61"/>
+    <mergeCell ref="H60:M61"/>
+    <mergeCell ref="N60:Q60"/>
+    <mergeCell ref="R60:Z60"/>
+    <mergeCell ref="N61:Q61"/>
+    <mergeCell ref="R61:U61"/>
+    <mergeCell ref="X61:Z61"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="L54:T54"/>
+    <mergeCell ref="V54:X54"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="L55:U57"/>
+    <mergeCell ref="W55:X55"/>
+    <mergeCell ref="H56:K56"/>
+    <mergeCell ref="H57:K57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="E58:I58"/>
+    <mergeCell ref="K58:T58"/>
+    <mergeCell ref="V58:W58"/>
+    <mergeCell ref="X58:Z58"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="H43:I43"/>
     <mergeCell ref="R43:Z43"/>
@@ -5377,83 +5284,143 @@
     <mergeCell ref="I52:J52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="N52:W52"/>
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="L54:T54"/>
-    <mergeCell ref="V54:X54"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="L55:U57"/>
-    <mergeCell ref="W55:X55"/>
-    <mergeCell ref="H56:K56"/>
-    <mergeCell ref="H57:K57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="E58:I58"/>
-    <mergeCell ref="K58:T58"/>
-    <mergeCell ref="V58:W58"/>
-    <mergeCell ref="X58:Z58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="K59:T59"/>
-    <mergeCell ref="V59:W59"/>
-    <mergeCell ref="X59:Z59"/>
-    <mergeCell ref="B60:G61"/>
-    <mergeCell ref="H60:M61"/>
-    <mergeCell ref="N60:Q60"/>
-    <mergeCell ref="R60:Z60"/>
-    <mergeCell ref="N61:Q61"/>
-    <mergeCell ref="R61:U61"/>
-    <mergeCell ref="X61:Z61"/>
-    <mergeCell ref="B62:G63"/>
-    <mergeCell ref="H62:M63"/>
-    <mergeCell ref="N62:Q62"/>
-    <mergeCell ref="R62:U62"/>
-    <mergeCell ref="X62:Z62"/>
-    <mergeCell ref="N63:Q63"/>
-    <mergeCell ref="R63:U63"/>
-    <mergeCell ref="X63:Z63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="N64:Q64"/>
-    <mergeCell ref="R64:U64"/>
-    <mergeCell ref="X64:Z64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="N65:Q65"/>
-    <mergeCell ref="R65:U65"/>
-    <mergeCell ref="X65:Z65"/>
-    <mergeCell ref="N66:Q66"/>
-    <mergeCell ref="R66:U66"/>
-    <mergeCell ref="X66:Z66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="J67:L67"/>
-    <mergeCell ref="N67:Q67"/>
-    <mergeCell ref="R67:U67"/>
-    <mergeCell ref="X67:Z67"/>
-    <mergeCell ref="N68:Q68"/>
-    <mergeCell ref="R68:U68"/>
-    <mergeCell ref="V68:W68"/>
-    <mergeCell ref="X68:Z68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="R69:Z69"/>
-    <mergeCell ref="B70:M70"/>
-    <mergeCell ref="N70:Z70"/>
-    <mergeCell ref="B71:M72"/>
-    <mergeCell ref="Q71:R71"/>
-    <mergeCell ref="Q72:R72"/>
-    <mergeCell ref="B73:D78"/>
-    <mergeCell ref="E73:M77"/>
-    <mergeCell ref="Q73:R73"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="N75:Z75"/>
-    <mergeCell ref="X77:Z77"/>
-    <mergeCell ref="E78:H78"/>
-    <mergeCell ref="I78:J78"/>
-    <mergeCell ref="K78:L78"/>
-    <mergeCell ref="N78:W78"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="N41:Q41"/>
+    <mergeCell ref="R41:U41"/>
+    <mergeCell ref="X41:Z41"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:U42"/>
+    <mergeCell ref="V42:W42"/>
+    <mergeCell ref="X42:Z42"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="N39:Q39"/>
+    <mergeCell ref="R39:U39"/>
+    <mergeCell ref="X39:Z39"/>
+    <mergeCell ref="N40:Q40"/>
+    <mergeCell ref="R40:U40"/>
+    <mergeCell ref="X40:Z40"/>
+    <mergeCell ref="B36:G37"/>
+    <mergeCell ref="H36:M37"/>
+    <mergeCell ref="N36:Q36"/>
+    <mergeCell ref="R36:U36"/>
+    <mergeCell ref="X36:Z36"/>
+    <mergeCell ref="N37:Q37"/>
+    <mergeCell ref="R37:U37"/>
+    <mergeCell ref="X37:Z37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="N38:Q38"/>
+    <mergeCell ref="R38:U38"/>
+    <mergeCell ref="X38:Z38"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="K33:T33"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="X33:Z33"/>
+    <mergeCell ref="B34:G35"/>
+    <mergeCell ref="H34:M35"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="R34:Z34"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="R35:U35"/>
+    <mergeCell ref="X35:Z35"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="L28:T28"/>
+    <mergeCell ref="V28:X28"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="L29:U31"/>
+    <mergeCell ref="W29:X29"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="K32:T32"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="X32:Z32"/>
+    <mergeCell ref="B19:M20"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="B21:D26"/>
+    <mergeCell ref="E21:M25"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="N23:Z23"/>
+    <mergeCell ref="X25:Z25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="N26:W26"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="R17:Z17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="N18:Z18"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="R14:U14"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="R15:U15"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="R12:U12"/>
+    <mergeCell ref="X12:Z12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="R13:U13"/>
+    <mergeCell ref="X13:Z13"/>
+    <mergeCell ref="B8:G9"/>
+    <mergeCell ref="H8:M9"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="R8:Z8"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="B10:G11"/>
+    <mergeCell ref="H10:M11"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="R10:U10"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="R11:U11"/>
+    <mergeCell ref="X11:Z11"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="K6:T6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="K7:T7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="B2:F5"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:T2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:U5"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -5468,7 +5435,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>